<commit_message>
encoding fixed, minor fixes, folder cleaned
</commit_message>
<xml_diff>
--- a/R2Q_Datensatz_leer.xlsx
+++ b/R2Q_Datensatz_leer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flemming\Google Drive\R\R2Q_App\R2Q_App_VCurrent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836E4EDF-2C5E-437C-B4C5-725AD983F35D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D680888F-D574-4606-B5C4-F29B6FDD366C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5010" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{9E668519-328E-4E8D-8980-09B3972F3278}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="204">
   <si>
     <t>Ressource</t>
   </si>
@@ -642,6 +642,9 @@
   </si>
   <si>
     <t>Sammelhinweis</t>
+  </si>
+  <si>
+    <t>uptime</t>
   </si>
 </sst>
 </file>
@@ -1344,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F27926E-B51A-449F-86DD-91CC7FF15C35}">
-  <dimension ref="A1:AA271"/>
+  <dimension ref="A1:AA273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15"/>
@@ -1397,7 +1400,7 @@
     </row>
     <row r="2" spans="1:12" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
       <c r="A2" s="40">
-        <f t="shared" ref="A2:A131" si="0">ROW(A2)-1</f>
+        <f t="shared" ref="A2:A133" si="0">ROW(A2)-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="40" t="s">
@@ -1498,24 +1501,22 @@
       <c r="C5" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>67</v>
-      </c>
+      <c r="D5" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" thickTop="1" thickBot="1">
       <c r="A6" s="40">
@@ -1532,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>96</v>
@@ -1562,7 +1563,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>96</v>
@@ -1592,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>96</v>
@@ -1618,11 +1619,11 @@
       <c r="C9" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>4</v>
+      <c r="E9" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>96</v>
@@ -1630,14 +1631,14 @@
       <c r="G9" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+    <row r="10" spans="1:12" ht="18.75" thickTop="1" thickBot="1">
       <c r="A10" s="40">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1648,52 +1649,52 @@
       <c r="C10" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A11" s="40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F11" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" s="18" t="s">
+      <c r="G11" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A11" s="40">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="39" t="s">
+      <c r="I11" s="6" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1715,7 +1716,7 @@
         <v>140</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>96</v>
@@ -1745,7 +1746,7 @@
         <v>140</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>96</v>
@@ -1771,11 +1772,11 @@
       <c r="D14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>2</v>
+      <c r="E14" s="20" t="s">
+        <v>140</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>96</v>
@@ -1783,8 +1784,8 @@
       <c r="H14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>69</v>
+      <c r="I14" s="39" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" thickTop="1" thickBot="1">
@@ -1805,7 +1806,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>96</v>
@@ -1835,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>96</v>
@@ -1865,7 +1866,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>96</v>
@@ -1895,7 +1896,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>96</v>
@@ -1925,7 +1926,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>96</v>
@@ -1955,7 +1956,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>96</v>
@@ -1981,11 +1982,11 @@
       <c r="D21" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>4</v>
+      <c r="E21" s="21" t="s">
+        <v>2</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>96</v>
@@ -1994,7 +1995,7 @@
         <v>7</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
@@ -2015,7 +2016,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>96</v>
@@ -2045,7 +2046,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>96</v>
@@ -2075,7 +2076,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>96</v>
@@ -2105,7 +2106,7 @@
         <v>4</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>96</v>
@@ -2117,7 +2118,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="26" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
       <c r="A26" s="40">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2135,7 +2136,7 @@
         <v>4</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>96</v>
@@ -2147,7 +2148,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+    <row r="27" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A27" s="40">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2161,11 +2162,11 @@
       <c r="D27" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="23" t="s">
-        <v>1</v>
+      <c r="E27" s="22" t="s">
+        <v>4</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>96</v>
@@ -2174,7 +2175,7 @@
         <v>7</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
@@ -2195,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>96</v>
@@ -2225,7 +2226,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>96</v>
@@ -2255,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>96</v>
@@ -2281,11 +2282,11 @@
       <c r="D31" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>3</v>
+      <c r="E31" s="23" t="s">
+        <v>1</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>96</v>
@@ -2294,10 +2295,10 @@
         <v>7</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
       <c r="A32" s="40">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2315,7 +2316,7 @@
         <v>3</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>96</v>
@@ -2327,7 +2328,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+    <row r="33" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A33" s="40">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2345,7 +2346,7 @@
         <v>3</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>96</v>
@@ -2375,7 +2376,7 @@
         <v>3</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>96</v>
@@ -2405,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>96</v>
@@ -2417,7 +2418,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="36" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
       <c r="A36" s="40">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2435,7 +2436,7 @@
         <v>3</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>96</v>
@@ -2447,7 +2448,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+    <row r="37" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A37" s="40">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2458,49 +2459,49 @@
       <c r="C37" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A38" s="40">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E38" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A38" s="40">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B38" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38" s="10" t="s">
+      <c r="F38" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H38" s="18" t="s">
         <v>7</v>
       </c>
       <c r="I38" s="6" t="s">
@@ -2522,7 +2523,7 @@
         <v>9</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>96</v>
@@ -2537,7 +2538,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+    <row r="40" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
       <c r="A40" s="40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2548,56 +2549,56 @@
       <c r="C40" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A41" s="40">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E41" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H40" s="18" t="s">
+      <c r="F41" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H41" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="I41" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:9" customFormat="1" ht="19.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A41" s="40">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="F41" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="G41" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H41" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="39" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+    <row r="42" spans="1:9" customFormat="1" ht="19.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A42" s="40">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2611,8 +2612,8 @@
       <c r="D42" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="26" t="s">
-        <v>62</v>
+      <c r="E42" s="23" t="s">
+        <v>116</v>
       </c>
       <c r="F42" s="27" t="s">
         <v>96</v>
@@ -2623,68 +2624,68 @@
       <c r="H42" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I42" s="11" t="s">
+      <c r="I42" s="39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A43" s="40">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H43" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A43" s="40">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D43" s="17" t="s">
+    <row r="44" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A44" s="40">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E44" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F43" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H43" s="18" t="s">
+      <c r="F44" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H44" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I43" s="6" t="s">
+      <c r="I44" s="6" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A44" s="40">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="F44" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H44" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
@@ -2702,7 +2703,7 @@
         <v>100</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F45" s="27" t="s">
         <v>96</v>
@@ -2714,70 +2715,70 @@
         <v>16</v>
       </c>
       <c r="I45" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A46" s="40">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G46" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H46" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="6" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A46" s="40">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D46" s="17" t="s">
+    <row r="47" spans="1:9" s="6" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A47" s="40">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E47" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F46" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H46" s="18" t="s">
+      <c r="F47" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H47" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="6" t="s">
+      <c r="I47" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A47" s="40">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F47" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="G47" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H47" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="I47" s="39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
+    <row r="48" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
       <c r="A48" s="40">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2792,7 +2793,7 @@
         <v>20</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F48" s="27" t="s">
         <v>96</v>
@@ -2807,7 +2808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+    <row r="49" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
       <c r="A49" s="40">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2819,82 +2820,82 @@
         <v>96</v>
       </c>
       <c r="D49" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H49" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A50" s="40">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="E49" s="29" t="s">
+      <c r="E50" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="G49" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H49" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I49" s="11" t="s">
+      <c r="F50" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G50" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H50" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="6" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A50" s="40">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D50" s="17" t="s">
+    <row r="51" spans="1:9" s="6" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A51" s="40">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G50" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H50" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" s="6" t="s">
+      <c r="E51" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="6" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A51" s="40">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B51" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -2912,109 +2913,109 @@
         <v>25</v>
       </c>
       <c r="E52" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A53" s="40">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="F52" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H52" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I52" s="6" t="s">
+      <c r="F53" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="6" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A53" s="40">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B53" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53" s="17" t="s">
+    <row r="54" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A54" s="40">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="6" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A55" s="40">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E55" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="F53" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G53" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H53" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I53" s="6" t="s">
+      <c r="F55" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="6" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="39" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A54" s="51">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B54" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D54" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E54" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="F54" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="G54" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="H54" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I54" s="39" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="39" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A55" s="51">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B55" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E55" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="F55" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="G55" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="H55" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="39" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="39" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
@@ -3032,7 +3033,7 @@
         <v>26</v>
       </c>
       <c r="E56" s="45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>96</v>
@@ -3062,7 +3063,7 @@
         <v>26</v>
       </c>
       <c r="E57" s="45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>96</v>
@@ -3092,7 +3093,7 @@
         <v>26</v>
       </c>
       <c r="E58" s="45" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>96</v>
@@ -3122,7 +3123,7 @@
         <v>26</v>
       </c>
       <c r="E59" s="45" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>96</v>
@@ -3152,7 +3153,7 @@
         <v>26</v>
       </c>
       <c r="E60" s="45" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>96</v>
@@ -3182,7 +3183,7 @@
         <v>26</v>
       </c>
       <c r="E61" s="45" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>96</v>
@@ -3212,7 +3213,7 @@
         <v>26</v>
       </c>
       <c r="E62" s="45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>96</v>
@@ -3242,7 +3243,7 @@
         <v>26</v>
       </c>
       <c r="E63" s="45" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>96</v>
@@ -3257,94 +3258,94 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A64" s="40">
+    <row r="64" spans="1:9" s="39" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A64" s="51">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="51" t="s">
         <v>98</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="D64" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="F64" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="G64" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="39" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A65" s="51">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="F65" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="G65" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H65" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A66" s="40">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D66" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="17" t="s">
+      <c r="E66" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="F64" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H64" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I64" s="6" t="s">
+      <c r="F66" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" s="6" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A65" s="40">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B65" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D65" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="E65" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="F65" s="48" t="s">
-        <v>123</v>
-      </c>
-      <c r="G65" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="H65" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I65" s="54" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A66" s="40">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B66" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D66" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="E66" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="F66" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="G66" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="H66" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" s="54" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3365,7 +3366,7 @@
         <v>177</v>
       </c>
       <c r="F67" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G67" s="48" t="s">
         <v>96</v>
@@ -3374,7 +3375,7 @@
         <v>13</v>
       </c>
       <c r="I67" s="54" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3395,7 +3396,7 @@
         <v>177</v>
       </c>
       <c r="F68" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G68" s="48" t="s">
         <v>96</v>
@@ -3404,7 +3405,7 @@
         <v>13</v>
       </c>
       <c r="I68" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3422,10 +3423,10 @@
         <v>118</v>
       </c>
       <c r="E69" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F69" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G69" s="48" t="s">
         <v>96</v>
@@ -3434,7 +3435,7 @@
         <v>13</v>
       </c>
       <c r="I69" s="54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3452,10 +3453,10 @@
         <v>118</v>
       </c>
       <c r="E70" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F70" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G70" s="48" t="s">
         <v>96</v>
@@ -3464,7 +3465,7 @@
         <v>13</v>
       </c>
       <c r="I70" s="54" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3485,7 +3486,7 @@
         <v>178</v>
       </c>
       <c r="F71" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G71" s="48" t="s">
         <v>96</v>
@@ -3494,7 +3495,7 @@
         <v>13</v>
       </c>
       <c r="I71" s="54" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3515,7 +3516,7 @@
         <v>178</v>
       </c>
       <c r="F72" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G72" s="48" t="s">
         <v>96</v>
@@ -3524,7 +3525,7 @@
         <v>13</v>
       </c>
       <c r="I72" s="54" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3542,10 +3543,10 @@
         <v>118</v>
       </c>
       <c r="E73" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F73" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G73" s="48" t="s">
         <v>96</v>
@@ -3554,7 +3555,7 @@
         <v>13</v>
       </c>
       <c r="I73" s="54" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3572,10 +3573,10 @@
         <v>118</v>
       </c>
       <c r="E74" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F74" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G74" s="48" t="s">
         <v>96</v>
@@ -3584,7 +3585,7 @@
         <v>13</v>
       </c>
       <c r="I74" s="54" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3605,7 +3606,7 @@
         <v>179</v>
       </c>
       <c r="F75" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G75" s="48" t="s">
         <v>96</v>
@@ -3614,7 +3615,7 @@
         <v>13</v>
       </c>
       <c r="I75" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3635,7 +3636,7 @@
         <v>179</v>
       </c>
       <c r="F76" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G76" s="48" t="s">
         <v>96</v>
@@ -3644,7 +3645,7 @@
         <v>13</v>
       </c>
       <c r="I76" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3662,10 +3663,10 @@
         <v>118</v>
       </c>
       <c r="E77" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F77" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G77" s="48" t="s">
         <v>96</v>
@@ -3674,7 +3675,7 @@
         <v>13</v>
       </c>
       <c r="I77" s="54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3692,10 +3693,10 @@
         <v>118</v>
       </c>
       <c r="E78" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F78" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G78" s="48" t="s">
         <v>96</v>
@@ -3704,7 +3705,7 @@
         <v>13</v>
       </c>
       <c r="I78" s="54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3725,7 +3726,7 @@
         <v>180</v>
       </c>
       <c r="F79" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G79" s="48" t="s">
         <v>96</v>
@@ -3734,7 +3735,7 @@
         <v>13</v>
       </c>
       <c r="I79" s="54" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3755,7 +3756,7 @@
         <v>180</v>
       </c>
       <c r="F80" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G80" s="48" t="s">
         <v>96</v>
@@ -3764,7 +3765,7 @@
         <v>13</v>
       </c>
       <c r="I80" s="54" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3782,10 +3783,10 @@
         <v>118</v>
       </c>
       <c r="E81" s="45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F81" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G81" s="48" t="s">
         <v>96</v>
@@ -3794,7 +3795,7 @@
         <v>13</v>
       </c>
       <c r="I81" s="54" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3812,10 +3813,10 @@
         <v>118</v>
       </c>
       <c r="E82" s="45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F82" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G82" s="48" t="s">
         <v>96</v>
@@ -3824,7 +3825,7 @@
         <v>13</v>
       </c>
       <c r="I82" s="54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3845,7 +3846,7 @@
         <v>181</v>
       </c>
       <c r="F83" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G83" s="48" t="s">
         <v>96</v>
@@ -3854,7 +3855,7 @@
         <v>13</v>
       </c>
       <c r="I83" s="54" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3875,7 +3876,7 @@
         <v>181</v>
       </c>
       <c r="F84" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G84" s="48" t="s">
         <v>96</v>
@@ -3884,7 +3885,7 @@
         <v>13</v>
       </c>
       <c r="I84" s="54" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3902,10 +3903,10 @@
         <v>118</v>
       </c>
       <c r="E85" s="45" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="F85" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G85" s="48" t="s">
         <v>96</v>
@@ -3914,7 +3915,7 @@
         <v>13</v>
       </c>
       <c r="I85" s="54" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3932,10 +3933,10 @@
         <v>118</v>
       </c>
       <c r="E86" s="45" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G86" s="48" t="s">
         <v>96</v>
@@ -3944,7 +3945,7 @@
         <v>13</v>
       </c>
       <c r="I86" s="54" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
     </row>
     <row r="87" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3965,7 +3966,7 @@
         <v>124</v>
       </c>
       <c r="F87" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G87" s="48" t="s">
         <v>96</v>
@@ -3974,7 +3975,7 @@
         <v>13</v>
       </c>
       <c r="I87" s="54" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -3995,7 +3996,7 @@
         <v>124</v>
       </c>
       <c r="F88" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G88" s="48" t="s">
         <v>96</v>
@@ -4004,7 +4005,7 @@
         <v>13</v>
       </c>
       <c r="I88" s="54" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="89" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4022,10 +4023,10 @@
         <v>118</v>
       </c>
       <c r="E89" s="45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F89" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G89" s="48" t="s">
         <v>96</v>
@@ -4034,7 +4035,7 @@
         <v>13</v>
       </c>
       <c r="I89" s="54" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4052,10 +4053,10 @@
         <v>118</v>
       </c>
       <c r="E90" s="45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F90" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G90" s="48" t="s">
         <v>96</v>
@@ -4064,7 +4065,7 @@
         <v>13</v>
       </c>
       <c r="I90" s="54" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4085,7 +4086,7 @@
         <v>125</v>
       </c>
       <c r="F91" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G91" s="48" t="s">
         <v>96</v>
@@ -4094,7 +4095,7 @@
         <v>13</v>
       </c>
       <c r="I91" s="54" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4115,7 +4116,7 @@
         <v>125</v>
       </c>
       <c r="F92" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G92" s="48" t="s">
         <v>96</v>
@@ -4124,7 +4125,7 @@
         <v>13</v>
       </c>
       <c r="I92" s="54" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4142,10 +4143,10 @@
         <v>118</v>
       </c>
       <c r="E93" s="45" t="s">
-        <v>182</v>
+        <v>125</v>
       </c>
       <c r="F93" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G93" s="48" t="s">
         <v>96</v>
@@ -4154,7 +4155,7 @@
         <v>13</v>
       </c>
       <c r="I93" s="54" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4172,10 +4173,10 @@
         <v>118</v>
       </c>
       <c r="E94" s="45" t="s">
-        <v>182</v>
+        <v>125</v>
       </c>
       <c r="F94" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G94" s="48" t="s">
         <v>96</v>
@@ -4184,7 +4185,7 @@
         <v>13</v>
       </c>
       <c r="I94" s="54" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4205,7 +4206,7 @@
         <v>182</v>
       </c>
       <c r="F95" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G95" s="48" t="s">
         <v>96</v>
@@ -4214,7 +4215,7 @@
         <v>13</v>
       </c>
       <c r="I95" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4235,7 +4236,7 @@
         <v>182</v>
       </c>
       <c r="F96" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G96" s="48" t="s">
         <v>96</v>
@@ -4244,7 +4245,7 @@
         <v>13</v>
       </c>
       <c r="I96" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4262,10 +4263,10 @@
         <v>118</v>
       </c>
       <c r="E97" s="45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F97" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G97" s="48" t="s">
         <v>96</v>
@@ -4274,7 +4275,7 @@
         <v>13</v>
       </c>
       <c r="I97" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="98" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4292,10 +4293,10 @@
         <v>118</v>
       </c>
       <c r="E98" s="45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F98" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G98" s="48" t="s">
         <v>96</v>
@@ -4304,7 +4305,7 @@
         <v>13</v>
       </c>
       <c r="I98" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4325,7 +4326,7 @@
         <v>183</v>
       </c>
       <c r="F99" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G99" s="48" t="s">
         <v>96</v>
@@ -4334,7 +4335,7 @@
         <v>13</v>
       </c>
       <c r="I99" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="100" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4355,7 +4356,7 @@
         <v>183</v>
       </c>
       <c r="F100" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G100" s="48" t="s">
         <v>96</v>
@@ -4364,7 +4365,7 @@
         <v>13</v>
       </c>
       <c r="I100" s="54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4382,10 +4383,10 @@
         <v>118</v>
       </c>
       <c r="E101" s="45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F101" s="48" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="G101" s="48" t="s">
         <v>96</v>
@@ -4394,7 +4395,7 @@
         <v>13</v>
       </c>
       <c r="I101" s="54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4412,10 +4413,10 @@
         <v>118</v>
       </c>
       <c r="E102" s="45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F102" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G102" s="48" t="s">
         <v>96</v>
@@ -4424,7 +4425,7 @@
         <v>13</v>
       </c>
       <c r="I102" s="54" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4445,7 +4446,7 @@
         <v>184</v>
       </c>
       <c r="F103" s="48" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="G103" s="48" t="s">
         <v>96</v>
@@ -4454,7 +4455,7 @@
         <v>13</v>
       </c>
       <c r="I103" s="54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4475,80 +4476,76 @@
         <v>184</v>
       </c>
       <c r="F104" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="G104" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H104" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I104" s="54" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A105" s="40">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="B105" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D105" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="E105" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="F105" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G105" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H105" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I105" s="54" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27" s="39" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A106" s="40">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="B106" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D106" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="E106" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="F106" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="G104" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="H104" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I104" s="54" t="s">
+      <c r="G106" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H106" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I106" s="54" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="105" spans="1:27" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A105" s="40">
-        <f t="shared" si="0"/>
-        <v>104</v>
-      </c>
-      <c r="B105" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D105" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="E105" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="F105" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G105" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I105" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="J105" s="53"/>
-    </row>
-    <row r="106" spans="1:27" s="39" customFormat="1" ht="61.5" thickTop="1" thickBot="1">
-      <c r="A106" s="51">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="B106" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D106" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="E106" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="F106" s="45">
-        <v>1</v>
-      </c>
-      <c r="G106" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="H106" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="I106" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="J106" s="45" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="107" spans="1:27" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -4562,49 +4559,32 @@
       <c r="C107" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D107" s="45" t="s">
+      <c r="D107" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E107" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="F107" s="45">
-        <v>2</v>
-      </c>
-      <c r="G107" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H107" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="I107" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="J107" s="39"/>
-      <c r="K107" s="39"/>
-      <c r="L107" s="39"/>
-      <c r="M107" s="39"/>
-      <c r="N107" s="39"/>
-      <c r="O107" s="39"/>
-      <c r="P107" s="39"/>
-      <c r="Q107" s="39"/>
-      <c r="R107" s="39"/>
-      <c r="S107" s="39"/>
-      <c r="T107" s="39"/>
-      <c r="U107" s="39"/>
-      <c r="V107" s="39"/>
-      <c r="W107" s="39"/>
-      <c r="X107" s="39"/>
-      <c r="Y107" s="39"/>
-      <c r="Z107" s="39"/>
-      <c r="AA107" s="39"/>
-    </row>
-    <row r="108" spans="1:27" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A108" s="40">
+      <c r="E107" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I107" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="J107" s="53"/>
+    </row>
+    <row r="108" spans="1:27" s="39" customFormat="1" ht="61.5" thickTop="1" thickBot="1">
+      <c r="A108" s="51">
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="B108" s="40" t="s">
+      <c r="B108" s="51" t="s">
         <v>98</v>
       </c>
       <c r="C108" s="7" t="s">
@@ -4617,9 +4597,9 @@
         <v>103</v>
       </c>
       <c r="F108" s="45">
-        <v>3</v>
-      </c>
-      <c r="G108" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G108" s="50" t="s">
         <v>96</v>
       </c>
       <c r="H108" s="48" t="s">
@@ -4628,24 +4608,9 @@
       <c r="I108" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="J108" s="39"/>
-      <c r="K108" s="39"/>
-      <c r="L108" s="39"/>
-      <c r="M108" s="39"/>
-      <c r="N108" s="39"/>
-      <c r="O108" s="39"/>
-      <c r="P108" s="39"/>
-      <c r="Q108" s="39"/>
-      <c r="R108" s="39"/>
-      <c r="S108" s="39"/>
-      <c r="T108" s="39"/>
-      <c r="U108" s="39"/>
-      <c r="V108" s="39"/>
-      <c r="W108" s="39"/>
-      <c r="X108" s="39"/>
-      <c r="Y108" s="39"/>
-      <c r="Z108" s="39"/>
-      <c r="AA108" s="39"/>
+      <c r="J108" s="45" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="109" spans="1:27" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
       <c r="A109" s="40">
@@ -4665,7 +4630,7 @@
         <v>103</v>
       </c>
       <c r="F109" s="45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G109" s="27" t="s">
         <v>96</v>
@@ -4713,7 +4678,7 @@
         <v>103</v>
       </c>
       <c r="F110" s="45">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G110" s="27" t="s">
         <v>96</v>
@@ -4761,7 +4726,7 @@
         <v>103</v>
       </c>
       <c r="F111" s="45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G111" s="27" t="s">
         <v>96</v>
@@ -4809,7 +4774,7 @@
         <v>103</v>
       </c>
       <c r="F112" s="45">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G112" s="27" t="s">
         <v>96</v>
@@ -4857,7 +4822,7 @@
         <v>103</v>
       </c>
       <c r="F113" s="45">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G113" s="27" t="s">
         <v>96</v>
@@ -4905,7 +4870,7 @@
         <v>103</v>
       </c>
       <c r="F114" s="45">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G114" s="27" t="s">
         <v>96</v>
@@ -4953,7 +4918,7 @@
         <v>103</v>
       </c>
       <c r="F115" s="45">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G115" s="27" t="s">
         <v>96</v>
@@ -4997,11 +4962,11 @@
       <c r="D116" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="E116" s="21" t="s">
-        <v>5</v>
+      <c r="E116" s="46" t="s">
+        <v>103</v>
       </c>
       <c r="F116" s="45">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G116" s="27" t="s">
         <v>96</v>
@@ -5045,11 +5010,11 @@
       <c r="D117" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="E117" s="21" t="s">
-        <v>5</v>
+      <c r="E117" s="46" t="s">
+        <v>103</v>
       </c>
       <c r="F117" s="45">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G117" s="27" t="s">
         <v>96</v>
@@ -5097,7 +5062,7 @@
         <v>5</v>
       </c>
       <c r="F118" s="45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G118" s="27" t="s">
         <v>96</v>
@@ -5145,7 +5110,7 @@
         <v>5</v>
       </c>
       <c r="F119" s="45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G119" s="27" t="s">
         <v>96</v>
@@ -5193,7 +5158,7 @@
         <v>5</v>
       </c>
       <c r="F120" s="45">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G120" s="27" t="s">
         <v>96</v>
@@ -5241,7 +5206,7 @@
         <v>5</v>
       </c>
       <c r="F121" s="45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G121" s="27" t="s">
         <v>96</v>
@@ -5289,7 +5254,7 @@
         <v>5</v>
       </c>
       <c r="F122" s="45">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G122" s="27" t="s">
         <v>96</v>
@@ -5337,7 +5302,7 @@
         <v>5</v>
       </c>
       <c r="F123" s="45">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G123" s="27" t="s">
         <v>96</v>
@@ -5385,7 +5350,7 @@
         <v>5</v>
       </c>
       <c r="F124" s="45">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G124" s="27" t="s">
         <v>96</v>
@@ -5433,7 +5398,7 @@
         <v>5</v>
       </c>
       <c r="F125" s="45">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G125" s="27" t="s">
         <v>96</v>
@@ -5463,7 +5428,7 @@
       <c r="Z125" s="39"/>
       <c r="AA125" s="39"/>
     </row>
-    <row r="126" spans="1:27" s="6" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
+    <row r="126" spans="1:27" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
       <c r="A126" s="40">
         <f t="shared" si="0"/>
         <v>125</v>
@@ -5474,83 +5439,119 @@
       <c r="C126" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D126" s="17" t="s">
+      <c r="D126" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E126" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F126" s="45">
+        <v>9</v>
+      </c>
+      <c r="G126" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H126" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I126" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="J126" s="39"/>
+      <c r="K126" s="39"/>
+      <c r="L126" s="39"/>
+      <c r="M126" s="39"/>
+      <c r="N126" s="39"/>
+      <c r="O126" s="39"/>
+      <c r="P126" s="39"/>
+      <c r="Q126" s="39"/>
+      <c r="R126" s="39"/>
+      <c r="S126" s="39"/>
+      <c r="T126" s="39"/>
+      <c r="U126" s="39"/>
+      <c r="V126" s="39"/>
+      <c r="W126" s="39"/>
+      <c r="X126" s="39"/>
+      <c r="Y126" s="39"/>
+      <c r="Z126" s="39"/>
+      <c r="AA126" s="39"/>
+    </row>
+    <row r="127" spans="1:27" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A127" s="40">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="B127" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D127" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E127" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F127" s="45">
+        <v>10</v>
+      </c>
+      <c r="G127" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H127" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I127" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="J127" s="39"/>
+      <c r="K127" s="39"/>
+      <c r="L127" s="39"/>
+      <c r="M127" s="39"/>
+      <c r="N127" s="39"/>
+      <c r="O127" s="39"/>
+      <c r="P127" s="39"/>
+      <c r="Q127" s="39"/>
+      <c r="R127" s="39"/>
+      <c r="S127" s="39"/>
+      <c r="T127" s="39"/>
+      <c r="U127" s="39"/>
+      <c r="V127" s="39"/>
+      <c r="W127" s="39"/>
+      <c r="X127" s="39"/>
+      <c r="Y127" s="39"/>
+      <c r="Z127" s="39"/>
+      <c r="AA127" s="39"/>
+    </row>
+    <row r="128" spans="1:27" s="6" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A128" s="40">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="B128" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D128" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E126" s="17" t="s">
+      <c r="E128" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F126" s="18" t="s">
+      <c r="F128" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="G126" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H126" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I126" s="6" t="s">
+      <c r="G128" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H128" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I128" s="6" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="127" spans="1:27" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A127" s="40">
-        <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="B127" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E127" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F127" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G127" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H127" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I127" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="128" spans="1:27" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A128" s="40">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="B128" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C128" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D128" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E128" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F128" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G128" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H128" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I128" s="11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
@@ -5571,7 +5572,7 @@
         <v>29</v>
       </c>
       <c r="F129" s="27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G129" s="27" t="s">
         <v>96</v>
@@ -5580,7 +5581,7 @@
         <v>13</v>
       </c>
       <c r="I129" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
@@ -5601,7 +5602,7 @@
         <v>29</v>
       </c>
       <c r="F130" s="27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G130" s="27" t="s">
         <v>96</v>
@@ -5610,7 +5611,7 @@
         <v>13</v>
       </c>
       <c r="I130" s="11" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
@@ -5631,7 +5632,7 @@
         <v>29</v>
       </c>
       <c r="F131" s="27" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="G131" s="27" t="s">
         <v>96</v>
@@ -5640,12 +5641,12 @@
         <v>13</v>
       </c>
       <c r="I131" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
       <c r="A132" s="40">
-        <f t="shared" ref="A132:A180" si="1">ROW(A132)-1</f>
+        <f t="shared" si="0"/>
         <v>131</v>
       </c>
       <c r="B132" s="40" t="s">
@@ -5657,11 +5658,11 @@
       <c r="D132" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E132" s="31" t="s">
-        <v>31</v>
+      <c r="E132" s="30" t="s">
+        <v>29</v>
       </c>
       <c r="F132" s="27" t="s">
-        <v>140</v>
+        <v>4</v>
       </c>
       <c r="G132" s="27" t="s">
         <v>96</v>
@@ -5670,12 +5671,12 @@
         <v>13</v>
       </c>
       <c r="I132" s="11" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
       <c r="A133" s="40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="B133" s="40" t="s">
@@ -5687,11 +5688,11 @@
       <c r="D133" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E133" s="31" t="s">
-        <v>31</v>
+      <c r="E133" s="30" t="s">
+        <v>29</v>
       </c>
       <c r="F133" s="27" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G133" s="27" t="s">
         <v>96</v>
@@ -5700,12 +5701,12 @@
         <v>13</v>
       </c>
       <c r="I133" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
       <c r="A134" s="40">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A134:A182" si="1">ROW(A134)-1</f>
         <v>133</v>
       </c>
       <c r="B134" s="40" t="s">
@@ -5721,7 +5722,7 @@
         <v>31</v>
       </c>
       <c r="F134" s="27" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="G134" s="27" t="s">
         <v>96</v>
@@ -5730,7 +5731,7 @@
         <v>13</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>90</v>
+        <v>143</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
@@ -5751,7 +5752,7 @@
         <v>31</v>
       </c>
       <c r="F135" s="27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G135" s="27" t="s">
         <v>96</v>
@@ -5760,7 +5761,7 @@
         <v>13</v>
       </c>
       <c r="I135" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
@@ -5781,7 +5782,7 @@
         <v>31</v>
       </c>
       <c r="F136" s="27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G136" s="27" t="s">
         <v>96</v>
@@ -5790,7 +5791,7 @@
         <v>13</v>
       </c>
       <c r="I136" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
@@ -5811,7 +5812,7 @@
         <v>31</v>
       </c>
       <c r="F137" s="27" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="G137" s="27" t="s">
         <v>96</v>
@@ -5820,10 +5821,10 @@
         <v>13</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
       <c r="A138" s="40">
         <f t="shared" si="1"/>
         <v>137</v>
@@ -5834,83 +5835,83 @@
       <c r="C138" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D138" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="E138" s="31">
-        <v>1</v>
-      </c>
-      <c r="F138" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="G138" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="H138" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I138" s="34" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A139" s="51">
+      <c r="D138" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E138" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F138" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G138" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H138" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I138" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A139" s="40">
         <f t="shared" si="1"/>
         <v>138</v>
       </c>
-      <c r="B139" s="51" t="s">
+      <c r="B139" s="40" t="s">
         <v>98</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D139" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="E139" s="49">
-        <v>2</v>
-      </c>
-      <c r="F139" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="G139" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="H139" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="I139" s="47" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A140" s="51">
+      <c r="D139" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E139" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F139" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G139" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H139" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I139" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A140" s="40">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
-      <c r="B140" s="51" t="s">
+      <c r="B140" s="40" t="s">
         <v>98</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D140" s="45" t="s">
+      <c r="D140" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="E140" s="49">
-        <v>3</v>
-      </c>
-      <c r="F140" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="G140" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="H140" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="I140" s="47" t="s">
-        <v>108</v>
+      <c r="E140" s="31">
+        <v>1</v>
+      </c>
+      <c r="F140" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="G140" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H140" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I140" s="34" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -5928,7 +5929,7 @@
         <v>64</v>
       </c>
       <c r="E141" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F141" s="49" t="s">
         <v>96</v>
@@ -5940,7 +5941,7 @@
         <v>13</v>
       </c>
       <c r="I141" s="47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="142" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -5958,7 +5959,7 @@
         <v>64</v>
       </c>
       <c r="E142" s="49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F142" s="49" t="s">
         <v>96</v>
@@ -5970,7 +5971,7 @@
         <v>13</v>
       </c>
       <c r="I142" s="47" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="143" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -5988,7 +5989,7 @@
         <v>64</v>
       </c>
       <c r="E143" s="49">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F143" s="49" t="s">
         <v>96</v>
@@ -6000,7 +6001,7 @@
         <v>13</v>
       </c>
       <c r="I143" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -6018,7 +6019,7 @@
         <v>64</v>
       </c>
       <c r="E144" s="49">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F144" s="49" t="s">
         <v>96</v>
@@ -6030,7 +6031,7 @@
         <v>13</v>
       </c>
       <c r="I144" s="47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="145" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -6048,7 +6049,7 @@
         <v>64</v>
       </c>
       <c r="E145" s="49">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F145" s="49" t="s">
         <v>96</v>
@@ -6060,7 +6061,7 @@
         <v>13</v>
       </c>
       <c r="I145" s="47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="146" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -6078,7 +6079,7 @@
         <v>64</v>
       </c>
       <c r="E146" s="49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F146" s="49" t="s">
         <v>96</v>
@@ -6090,7 +6091,7 @@
         <v>13</v>
       </c>
       <c r="I146" s="47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="147" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
@@ -6108,7 +6109,7 @@
         <v>64</v>
       </c>
       <c r="E147" s="49">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F147" s="49" t="s">
         <v>96</v>
@@ -6120,70 +6121,70 @@
         <v>13</v>
       </c>
       <c r="I147" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" s="34" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A148" s="40">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A148" s="51">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
-      <c r="B148" s="40" t="s">
+      <c r="B148" s="51" t="s">
         <v>98</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D148" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E148" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F148" s="33">
-        <v>1</v>
-      </c>
-      <c r="G148" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H148" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I148" s="34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A149" s="40">
+      <c r="D148" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E148" s="49">
+        <v>9</v>
+      </c>
+      <c r="F148" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="G148" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="H148" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="I148" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A149" s="51">
         <f t="shared" si="1"/>
         <v>148</v>
       </c>
-      <c r="B149" s="40" t="s">
+      <c r="B149" s="51" t="s">
         <v>98</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D149" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E149" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F149" s="27">
-        <v>2</v>
-      </c>
-      <c r="G149" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H149" s="27" t="s">
+      <c r="D149" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E149" s="49">
+        <v>10</v>
+      </c>
+      <c r="F149" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="G149" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="H149" s="50" t="s">
         <v>13</v>
       </c>
       <c r="I149" s="47" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" s="34" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
       <c r="A150" s="40">
         <f t="shared" si="1"/>
         <v>149</v>
@@ -6194,22 +6195,22 @@
       <c r="C150" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D150" s="8" t="s">
+      <c r="D150" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E150" s="35" t="s">
+      <c r="E150" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F150" s="27">
-        <v>3</v>
-      </c>
-      <c r="G150" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H150" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I150" s="47" t="s">
+      <c r="F150" s="33">
+        <v>1</v>
+      </c>
+      <c r="G150" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H150" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I150" s="34" t="s">
         <v>105</v>
       </c>
     </row>
@@ -6231,7 +6232,7 @@
         <v>34</v>
       </c>
       <c r="F151" s="27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G151" s="27" t="s">
         <v>96</v>
@@ -6261,7 +6262,7 @@
         <v>34</v>
       </c>
       <c r="F152" s="27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G152" s="27" t="s">
         <v>96</v>
@@ -6291,7 +6292,7 @@
         <v>34</v>
       </c>
       <c r="F153" s="27">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G153" s="27" t="s">
         <v>96</v>
@@ -6321,7 +6322,7 @@
         <v>34</v>
       </c>
       <c r="F154" s="27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G154" s="27" t="s">
         <v>96</v>
@@ -6351,7 +6352,7 @@
         <v>34</v>
       </c>
       <c r="F155" s="27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G155" s="27" t="s">
         <v>96</v>
@@ -6381,7 +6382,7 @@
         <v>34</v>
       </c>
       <c r="F156" s="27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G156" s="27" t="s">
         <v>96</v>
@@ -6411,7 +6412,7 @@
         <v>34</v>
       </c>
       <c r="F157" s="27">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G157" s="27" t="s">
         <v>96</v>
@@ -6423,7 +6424,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="158" spans="1:9" s="34" customFormat="1" ht="61.5" customHeight="1" thickTop="1" thickBot="1">
+    <row r="158" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
       <c r="A158" s="40">
         <f t="shared" si="1"/>
         <v>157</v>
@@ -6434,22 +6435,22 @@
       <c r="C158" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D158" s="32" t="s">
+      <c r="D158" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E158" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="F158" s="33">
-        <v>1</v>
-      </c>
-      <c r="G158" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H158" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I158" s="34" t="s">
+      <c r="E158" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F158" s="27">
+        <v>9</v>
+      </c>
+      <c r="G158" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H158" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I158" s="47" t="s">
         <v>105</v>
       </c>
     </row>
@@ -6467,11 +6468,11 @@
       <c r="D159" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E159" s="36" t="s">
-        <v>35</v>
+      <c r="E159" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="F159" s="27">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G159" s="27" t="s">
         <v>96</v>
@@ -6483,7 +6484,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+    <row r="160" spans="1:9" s="34" customFormat="1" ht="61.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A160" s="40">
         <f t="shared" si="1"/>
         <v>159</v>
@@ -6494,22 +6495,22 @@
       <c r="C160" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D160" s="8" t="s">
+      <c r="D160" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E160" s="36" t="s">
+      <c r="E160" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F160" s="27">
-        <v>3</v>
-      </c>
-      <c r="G160" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="H160" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I160" s="47" t="s">
+      <c r="F160" s="33">
+        <v>1</v>
+      </c>
+      <c r="G160" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H160" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I160" s="34" t="s">
         <v>105</v>
       </c>
     </row>
@@ -6531,7 +6532,7 @@
         <v>35</v>
       </c>
       <c r="F161" s="27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G161" s="27" t="s">
         <v>96</v>
@@ -6561,7 +6562,7 @@
         <v>35</v>
       </c>
       <c r="F162" s="27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G162" s="27" t="s">
         <v>96</v>
@@ -6591,7 +6592,7 @@
         <v>35</v>
       </c>
       <c r="F163" s="27">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G163" s="27" t="s">
         <v>96</v>
@@ -6621,7 +6622,7 @@
         <v>35</v>
       </c>
       <c r="F164" s="27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G164" s="27" t="s">
         <v>96</v>
@@ -6651,7 +6652,7 @@
         <v>35</v>
       </c>
       <c r="F165" s="27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G165" s="27" t="s">
         <v>96</v>
@@ -6681,7 +6682,7 @@
         <v>35</v>
       </c>
       <c r="F166" s="27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G166" s="27" t="s">
         <v>96</v>
@@ -6711,7 +6712,7 @@
         <v>35</v>
       </c>
       <c r="F167" s="27">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G167" s="27" t="s">
         <v>96</v>
@@ -6723,7 +6724,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="168" spans="1:9" s="34" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+    <row r="168" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
       <c r="A168" s="40">
         <f t="shared" si="1"/>
         <v>167</v>
@@ -6734,82 +6735,82 @@
       <c r="C168" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D168" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="E168" s="31">
-        <v>1</v>
-      </c>
-      <c r="F168" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="G168" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H168" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I168" s="34" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A169" s="51">
+      <c r="D168" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E168" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F168" s="27">
+        <v>9</v>
+      </c>
+      <c r="G168" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H168" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I168" s="47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A169" s="40">
         <f t="shared" si="1"/>
         <v>168</v>
       </c>
-      <c r="B169" s="51" t="s">
+      <c r="B169" s="40" t="s">
         <v>98</v>
       </c>
       <c r="C169" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D169" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="E169" s="49">
-        <v>1</v>
-      </c>
-      <c r="F169" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="G169" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="H169" s="50" t="s">
+      <c r="D169" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E169" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F169" s="27">
+        <v>10</v>
+      </c>
+      <c r="G169" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H169" s="27" t="s">
         <v>13</v>
       </c>
       <c r="I169" s="47" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A170" s="51">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" s="34" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A170" s="40">
         <f t="shared" si="1"/>
         <v>169</v>
       </c>
-      <c r="B170" s="51" t="s">
+      <c r="B170" s="40" t="s">
         <v>98</v>
       </c>
       <c r="C170" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D170" s="45" t="s">
+      <c r="D170" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="E170" s="49">
+      <c r="E170" s="31">
         <v>1</v>
       </c>
-      <c r="F170" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="G170" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="H170" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="I170" s="47" t="s">
+      <c r="F170" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="G170" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H170" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I170" s="34" t="s">
         <v>134</v>
       </c>
     </row>
@@ -6831,7 +6832,7 @@
         <v>1</v>
       </c>
       <c r="F171" s="49" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G171" s="49" t="s">
         <v>96</v>
@@ -6858,10 +6859,10 @@
         <v>121</v>
       </c>
       <c r="E172" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F172" s="49" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G172" s="49" t="s">
         <v>96</v>
@@ -6888,10 +6889,10 @@
         <v>121</v>
       </c>
       <c r="E173" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F173" s="49" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G173" s="49" t="s">
         <v>96</v>
@@ -6921,7 +6922,7 @@
         <v>2</v>
       </c>
       <c r="F174" s="49" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G174" s="49" t="s">
         <v>96</v>
@@ -6951,7 +6952,7 @@
         <v>2</v>
       </c>
       <c r="F175" s="49" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G175" s="49" t="s">
         <v>96</v>
@@ -6978,10 +6979,10 @@
         <v>121</v>
       </c>
       <c r="E176" s="49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F176" s="49" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G176" s="49" t="s">
         <v>96</v>
@@ -7008,10 +7009,10 @@
         <v>121</v>
       </c>
       <c r="E177" s="49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F177" s="49" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G177" s="49" t="s">
         <v>96</v>
@@ -7041,7 +7042,7 @@
         <v>3</v>
       </c>
       <c r="F178" s="49" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G178" s="49" t="s">
         <v>96</v>
@@ -7071,7 +7072,7 @@
         <v>3</v>
       </c>
       <c r="F179" s="49" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G179" s="49" t="s">
         <v>96</v>
@@ -7083,45 +7084,97 @@
         <v>134</v>
       </c>
     </row>
-    <row r="180" spans="1:9" s="34" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
-      <c r="A180" s="40">
+    <row r="180" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A180" s="51">
         <f t="shared" si="1"/>
         <v>179</v>
       </c>
-      <c r="B180" s="40" t="s">
+      <c r="B180" s="51" t="s">
         <v>98</v>
       </c>
       <c r="C180" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D180" s="32" t="s">
+      <c r="D180" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="E180" s="49">
+        <v>3</v>
+      </c>
+      <c r="F180" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="G180" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="H180" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="I180" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" s="47" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A181" s="51">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="B181" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D181" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="E181" s="49">
+        <v>3</v>
+      </c>
+      <c r="F181" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="G181" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="H181" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="I181" s="47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" s="34" customFormat="1" ht="18.75" thickTop="1" thickBot="1">
+      <c r="A182" s="40">
+        <f t="shared" si="1"/>
+        <v>181</v>
+      </c>
+      <c r="B182" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C182" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D182" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E180" s="31" t="s">
+      <c r="E182" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="F180" s="31" t="s">
+      <c r="F182" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="G180" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="H180" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I180" s="34" t="s">
+      <c r="G182" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H182" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I182" s="34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="15.75" thickTop="1">
-      <c r="D181" s="11"/>
-      <c r="E181" s="11"/>
-    </row>
-    <row r="182" spans="1:9">
-      <c r="D182" s="11"/>
-      <c r="E182" s="11"/>
-    </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" ht="15.75" thickTop="1">
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
     </row>
@@ -7477,10 +7530,18 @@
       <c r="D271" s="11"/>
       <c r="E271" s="11"/>
     </row>
+    <row r="272" spans="4:5">
+      <c r="D272" s="11"/>
+      <c r="E272" s="11"/>
+    </row>
+    <row r="273" spans="4:5">
+      <c r="D273" s="11"/>
+      <c r="E273" s="11"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G46:G48 G5:G39" xr:uid="{1F03BB8B-042F-4A2F-9E83-B52FD12070A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G47:G49 G6:G40" xr:uid="{1F03BB8B-042F-4A2F-9E83-B52FD12070A9}">
       <formula1>$A$2:$C$2</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added field "Hinweis" in section "Aufwand und Kosten"
</commit_message>
<xml_diff>
--- a/R2Q_Datensatz_leer.xlsx
+++ b/R2Q_Datensatz_leer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pramit\Documents\work\R2Q-Shiny-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D781CE-A465-4674-8F7D-98C55527BADC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8907AFAC-6A8A-4881-864E-770D6CADD401}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E668519-328E-4E8D-8980-09B3972F3278}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="208">
   <si>
     <t>Ressource</t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t>titel</t>
+  </si>
+  <si>
+    <t>kosten_hinweis</t>
   </si>
 </sst>
 </file>
@@ -1427,10 +1430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F27926E-B51A-449F-86DD-91CC7FF15C35}">
-  <dimension ref="A1:AA294"/>
+  <dimension ref="A1:AA295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E143" sqref="E143"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,7 +1483,7 @@
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="38">
-        <f t="shared" ref="A2:A154" si="0">ROW(A2)-1</f>
+        <f t="shared" ref="A2:A155" si="0">ROW(A2)-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
@@ -4658,9 +4661,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="108" spans="1:27" s="4" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:27" s="37" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="38">
-        <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="B108" s="38" t="s">
@@ -4669,65 +4671,62 @@
       <c r="C108" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D108" s="30" t="s">
+      <c r="D108" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="E108" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="G108" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="H108" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I108" s="52" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" s="4" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="38">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="B109" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D109" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E108" s="30" t="s">
+      <c r="E109" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="F108" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G108" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H108" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I108" s="50" t="s">
+      <c r="F109" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H109" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I109" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="J108" s="51"/>
-    </row>
-    <row r="109" spans="1:27" s="37" customFormat="1" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="49">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="B109" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D109" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="E109" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="F109" s="43">
-        <v>1</v>
-      </c>
-      <c r="G109" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="H109" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="I109" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="J109" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="110" spans="1:27" s="4" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="38">
+      <c r="J109" s="51"/>
+    </row>
+    <row r="110" spans="1:27" s="37" customFormat="1" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="49">
         <f t="shared" si="0"/>
         <v>109</v>
       </c>
-      <c r="B110" s="38" t="s">
+      <c r="B110" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C110" s="5" t="s">
@@ -4740,9 +4739,9 @@
         <v>103</v>
       </c>
       <c r="F110" s="43">
-        <v>2</v>
-      </c>
-      <c r="G110" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G110" s="48" t="s">
         <v>96</v>
       </c>
       <c r="H110" s="46" t="s">
@@ -4751,24 +4750,9 @@
       <c r="I110" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="J110" s="37"/>
-      <c r="K110" s="37"/>
-      <c r="L110" s="37"/>
-      <c r="M110" s="37"/>
-      <c r="N110" s="37"/>
-      <c r="O110" s="37"/>
-      <c r="P110" s="37"/>
-      <c r="Q110" s="37"/>
-      <c r="R110" s="37"/>
-      <c r="S110" s="37"/>
-      <c r="T110" s="37"/>
-      <c r="U110" s="37"/>
-      <c r="V110" s="37"/>
-      <c r="W110" s="37"/>
-      <c r="X110" s="37"/>
-      <c r="Y110" s="37"/>
-      <c r="Z110" s="37"/>
-      <c r="AA110" s="37"/>
+      <c r="J110" s="43" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="111" spans="1:27" s="4" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="38">
@@ -4788,7 +4772,7 @@
         <v>103</v>
       </c>
       <c r="F111" s="43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G111" s="25" t="s">
         <v>96</v>
@@ -4836,7 +4820,7 @@
         <v>103</v>
       </c>
       <c r="F112" s="43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G112" s="25" t="s">
         <v>96</v>
@@ -4884,7 +4868,7 @@
         <v>103</v>
       </c>
       <c r="F113" s="43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G113" s="25" t="s">
         <v>96</v>
@@ -4932,7 +4916,7 @@
         <v>103</v>
       </c>
       <c r="F114" s="43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G114" s="25" t="s">
         <v>96</v>
@@ -4980,7 +4964,7 @@
         <v>103</v>
       </c>
       <c r="F115" s="43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G115" s="25" t="s">
         <v>96</v>
@@ -5028,7 +5012,7 @@
         <v>103</v>
       </c>
       <c r="F116" s="43">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G116" s="25" t="s">
         <v>96</v>
@@ -5076,7 +5060,7 @@
         <v>103</v>
       </c>
       <c r="F117" s="43">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G117" s="25" t="s">
         <v>96</v>
@@ -5124,7 +5108,7 @@
         <v>103</v>
       </c>
       <c r="F118" s="43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G118" s="25" t="s">
         <v>96</v>
@@ -5154,12 +5138,12 @@
       <c r="Z118" s="37"/>
       <c r="AA118" s="37"/>
     </row>
-    <row r="119" spans="1:27" s="37" customFormat="1" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="49">
+    <row r="119" spans="1:27" s="4" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="38">
         <f t="shared" si="0"/>
         <v>118</v>
       </c>
-      <c r="B119" s="49" t="s">
+      <c r="B119" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C119" s="5" t="s">
@@ -5172,9 +5156,9 @@
         <v>103</v>
       </c>
       <c r="F119" s="43">
-        <v>11</v>
-      </c>
-      <c r="G119" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="G119" s="25" t="s">
         <v>96</v>
       </c>
       <c r="H119" s="46" t="s">
@@ -5183,16 +5167,31 @@
       <c r="I119" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="J119" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="120" spans="1:27" s="4" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="38">
+      <c r="J119" s="37"/>
+      <c r="K119" s="37"/>
+      <c r="L119" s="37"/>
+      <c r="M119" s="37"/>
+      <c r="N119" s="37"/>
+      <c r="O119" s="37"/>
+      <c r="P119" s="37"/>
+      <c r="Q119" s="37"/>
+      <c r="R119" s="37"/>
+      <c r="S119" s="37"/>
+      <c r="T119" s="37"/>
+      <c r="U119" s="37"/>
+      <c r="V119" s="37"/>
+      <c r="W119" s="37"/>
+      <c r="X119" s="37"/>
+      <c r="Y119" s="37"/>
+      <c r="Z119" s="37"/>
+      <c r="AA119" s="37"/>
+    </row>
+    <row r="120" spans="1:27" s="37" customFormat="1" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="49">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="B120" s="38" t="s">
+      <c r="B120" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C120" s="5" t="s">
@@ -5205,9 +5204,9 @@
         <v>103</v>
       </c>
       <c r="F120" s="43">
-        <v>12</v>
-      </c>
-      <c r="G120" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G120" s="48" t="s">
         <v>96</v>
       </c>
       <c r="H120" s="46" t="s">
@@ -5216,24 +5215,9 @@
       <c r="I120" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="J120" s="37"/>
-      <c r="K120" s="37"/>
-      <c r="L120" s="37"/>
-      <c r="M120" s="37"/>
-      <c r="N120" s="37"/>
-      <c r="O120" s="37"/>
-      <c r="P120" s="37"/>
-      <c r="Q120" s="37"/>
-      <c r="R120" s="37"/>
-      <c r="S120" s="37"/>
-      <c r="T120" s="37"/>
-      <c r="U120" s="37"/>
-      <c r="V120" s="37"/>
-      <c r="W120" s="37"/>
-      <c r="X120" s="37"/>
-      <c r="Y120" s="37"/>
-      <c r="Z120" s="37"/>
-      <c r="AA120" s="37"/>
+      <c r="J120" s="43" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="121" spans="1:27" s="4" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="38">
@@ -5253,7 +5237,7 @@
         <v>103</v>
       </c>
       <c r="F121" s="43">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G121" s="25" t="s">
         <v>96</v>
@@ -5301,7 +5285,7 @@
         <v>103</v>
       </c>
       <c r="F122" s="43">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G122" s="25" t="s">
         <v>96</v>
@@ -5349,7 +5333,7 @@
         <v>103</v>
       </c>
       <c r="F123" s="43">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G123" s="25" t="s">
         <v>96</v>
@@ -5397,7 +5381,7 @@
         <v>103</v>
       </c>
       <c r="F124" s="43">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G124" s="25" t="s">
         <v>96</v>
@@ -5445,7 +5429,7 @@
         <v>103</v>
       </c>
       <c r="F125" s="43">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G125" s="25" t="s">
         <v>96</v>
@@ -5493,7 +5477,7 @@
         <v>103</v>
       </c>
       <c r="F126" s="43">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G126" s="25" t="s">
         <v>96</v>
@@ -5541,7 +5525,7 @@
         <v>103</v>
       </c>
       <c r="F127" s="43">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G127" s="25" t="s">
         <v>96</v>
@@ -5589,7 +5573,7 @@
         <v>103</v>
       </c>
       <c r="F128" s="43">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G128" s="25" t="s">
         <v>96</v>
@@ -5633,11 +5617,11 @@
       <c r="D129" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="E129" s="19" t="s">
-        <v>5</v>
+      <c r="E129" s="44" t="s">
+        <v>103</v>
       </c>
       <c r="F129" s="43">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G129" s="25" t="s">
         <v>96</v>
@@ -5685,7 +5669,7 @@
         <v>5</v>
       </c>
       <c r="F130" s="43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G130" s="25" t="s">
         <v>96</v>
@@ -5733,7 +5717,7 @@
         <v>5</v>
       </c>
       <c r="F131" s="43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G131" s="25" t="s">
         <v>96</v>
@@ -5781,7 +5765,7 @@
         <v>5</v>
       </c>
       <c r="F132" s="43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G132" s="25" t="s">
         <v>96</v>
@@ -5829,7 +5813,7 @@
         <v>5</v>
       </c>
       <c r="F133" s="43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G133" s="25" t="s">
         <v>96</v>
@@ -5877,7 +5861,7 @@
         <v>5</v>
       </c>
       <c r="F134" s="43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G134" s="25" t="s">
         <v>96</v>
@@ -5925,7 +5909,7 @@
         <v>5</v>
       </c>
       <c r="F135" s="43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G135" s="25" t="s">
         <v>96</v>
@@ -5973,7 +5957,7 @@
         <v>5</v>
       </c>
       <c r="F136" s="43">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G136" s="25" t="s">
         <v>96</v>
@@ -6021,7 +6005,7 @@
         <v>5</v>
       </c>
       <c r="F137" s="43">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G137" s="25" t="s">
         <v>96</v>
@@ -6069,7 +6053,7 @@
         <v>5</v>
       </c>
       <c r="F138" s="43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G138" s="25" t="s">
         <v>96</v>
@@ -6117,7 +6101,7 @@
         <v>5</v>
       </c>
       <c r="F139" s="43">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G139" s="25" t="s">
         <v>96</v>
@@ -6165,7 +6149,7 @@
         <v>5</v>
       </c>
       <c r="F140" s="43">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G140" s="25" t="s">
         <v>96</v>
@@ -6213,7 +6197,7 @@
         <v>5</v>
       </c>
       <c r="F141" s="43">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G141" s="25" t="s">
         <v>96</v>
@@ -6261,7 +6245,7 @@
         <v>5</v>
       </c>
       <c r="F142" s="43">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G142" s="25" t="s">
         <v>96</v>
@@ -6309,7 +6293,7 @@
         <v>5</v>
       </c>
       <c r="F143" s="43">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G143" s="25" t="s">
         <v>96</v>
@@ -6357,7 +6341,7 @@
         <v>5</v>
       </c>
       <c r="F144" s="43">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G144" s="25" t="s">
         <v>96</v>
@@ -6405,7 +6389,7 @@
         <v>5</v>
       </c>
       <c r="F145" s="43">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G145" s="25" t="s">
         <v>96</v>
@@ -6453,7 +6437,7 @@
         <v>5</v>
       </c>
       <c r="F146" s="43">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G146" s="25" t="s">
         <v>96</v>
@@ -6501,7 +6485,7 @@
         <v>5</v>
       </c>
       <c r="F147" s="43">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G147" s="25" t="s">
         <v>96</v>
@@ -6549,7 +6533,7 @@
         <v>5</v>
       </c>
       <c r="F148" s="43">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G148" s="25" t="s">
         <v>96</v>
@@ -6590,53 +6574,71 @@
       <c r="C149" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D149" s="15" t="s">
+      <c r="D149" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E149" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F149" s="43">
+        <v>20</v>
+      </c>
+      <c r="G149" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H149" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I149" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="J149" s="37"/>
+      <c r="K149" s="37"/>
+      <c r="L149" s="37"/>
+      <c r="M149" s="37"/>
+      <c r="N149" s="37"/>
+      <c r="O149" s="37"/>
+      <c r="P149" s="37"/>
+      <c r="Q149" s="37"/>
+      <c r="R149" s="37"/>
+      <c r="S149" s="37"/>
+      <c r="T149" s="37"/>
+      <c r="U149" s="37"/>
+      <c r="V149" s="37"/>
+      <c r="W149" s="37"/>
+      <c r="X149" s="37"/>
+      <c r="Y149" s="37"/>
+      <c r="Z149" s="37"/>
+      <c r="AA149" s="37"/>
+    </row>
+    <row r="150" spans="1:27" s="4" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="38">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="B150" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D150" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E149" s="15" t="s">
+      <c r="E150" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F149" s="16" t="s">
+      <c r="F150" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="G149" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="H149" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I149" s="4" t="s">
+      <c r="G150" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H150" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I150" s="4" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="150" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="38">
-        <f t="shared" si="0"/>
-        <v>149</v>
-      </c>
-      <c r="B150" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="C150" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D150" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E150" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="F150" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="G150" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H150" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I150" s="9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="151" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6657,7 +6659,7 @@
         <v>29</v>
       </c>
       <c r="F151" s="25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G151" s="25" t="s">
         <v>96</v>
@@ -6666,7 +6668,7 @@
         <v>13</v>
       </c>
       <c r="I151" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="152" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6687,7 +6689,7 @@
         <v>29</v>
       </c>
       <c r="F152" s="25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G152" s="25" t="s">
         <v>96</v>
@@ -6696,7 +6698,7 @@
         <v>13</v>
       </c>
       <c r="I152" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="153" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6717,7 +6719,7 @@
         <v>29</v>
       </c>
       <c r="F153" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G153" s="25" t="s">
         <v>96</v>
@@ -6726,7 +6728,7 @@
         <v>13</v>
       </c>
       <c r="I153" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="154" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6747,7 +6749,7 @@
         <v>29</v>
       </c>
       <c r="F154" s="25" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G154" s="25" t="s">
         <v>96</v>
@@ -6756,12 +6758,12 @@
         <v>13</v>
       </c>
       <c r="I154" s="9" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="155" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="38">
-        <f t="shared" ref="A155:A203" si="1">ROW(A155)-1</f>
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="B155" s="38" t="s">
@@ -6773,11 +6775,11 @@
       <c r="D155" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E155" s="29" t="s">
-        <v>31</v>
+      <c r="E155" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="F155" s="25" t="s">
-        <v>140</v>
+        <v>30</v>
       </c>
       <c r="G155" s="25" t="s">
         <v>96</v>
@@ -6786,12 +6788,12 @@
         <v>13</v>
       </c>
       <c r="I155" s="9" t="s">
-        <v>143</v>
+        <v>88</v>
       </c>
     </row>
     <row r="156" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A156:A204" si="1">ROW(A156)-1</f>
         <v>155</v>
       </c>
       <c r="B156" s="38" t="s">
@@ -6807,7 +6809,7 @@
         <v>31</v>
       </c>
       <c r="F156" s="25" t="s">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="G156" s="25" t="s">
         <v>96</v>
@@ -6816,7 +6818,7 @@
         <v>13</v>
       </c>
       <c r="I156" s="9" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
     </row>
     <row r="157" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6837,7 +6839,7 @@
         <v>31</v>
       </c>
       <c r="F157" s="25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G157" s="25" t="s">
         <v>96</v>
@@ -6846,7 +6848,7 @@
         <v>13</v>
       </c>
       <c r="I157" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="158" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6867,7 +6869,7 @@
         <v>31</v>
       </c>
       <c r="F158" s="25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G158" s="25" t="s">
         <v>96</v>
@@ -6876,7 +6878,7 @@
         <v>13</v>
       </c>
       <c r="I158" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="159" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6897,7 +6899,7 @@
         <v>31</v>
       </c>
       <c r="F159" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G159" s="25" t="s">
         <v>96</v>
@@ -6906,7 +6908,7 @@
         <v>13</v>
       </c>
       <c r="I159" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="160" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6927,7 +6929,7 @@
         <v>31</v>
       </c>
       <c r="F160" s="25" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G160" s="25" t="s">
         <v>96</v>
@@ -6936,7 +6938,7 @@
         <v>13</v>
       </c>
       <c r="I160" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6950,53 +6952,53 @@
       <c r="C161" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D161" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E161" s="29">
-        <v>1</v>
-      </c>
-      <c r="F161" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="G161" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H161" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I161" s="32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="49">
+      <c r="D161" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E161" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F161" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G161" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H161" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I161" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="38">
         <f t="shared" si="1"/>
         <v>161</v>
       </c>
-      <c r="B162" s="49" t="s">
+      <c r="B162" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C162" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D162" s="43" t="s">
+      <c r="D162" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E162" s="47">
-        <v>2</v>
-      </c>
-      <c r="F162" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="G162" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="H162" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="I162" s="45" t="s">
-        <v>107</v>
+      <c r="E162" s="29">
+        <v>1</v>
+      </c>
+      <c r="F162" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="G162" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H162" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I162" s="32" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="163" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7014,7 +7016,7 @@
         <v>64</v>
       </c>
       <c r="E163" s="47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F163" s="47" t="s">
         <v>96</v>
@@ -7026,7 +7028,7 @@
         <v>13</v>
       </c>
       <c r="I163" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="164" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7044,7 +7046,7 @@
         <v>64</v>
       </c>
       <c r="E164" s="47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F164" s="47" t="s">
         <v>96</v>
@@ -7056,7 +7058,7 @@
         <v>13</v>
       </c>
       <c r="I164" s="45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="165" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7074,7 +7076,7 @@
         <v>64</v>
       </c>
       <c r="E165" s="47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F165" s="47" t="s">
         <v>96</v>
@@ -7086,7 +7088,7 @@
         <v>13</v>
       </c>
       <c r="I165" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="166" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7104,7 +7106,7 @@
         <v>64</v>
       </c>
       <c r="E166" s="47">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F166" s="47" t="s">
         <v>96</v>
@@ -7116,7 +7118,7 @@
         <v>13</v>
       </c>
       <c r="I166" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="167" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7134,7 +7136,7 @@
         <v>64</v>
       </c>
       <c r="E167" s="47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F167" s="47" t="s">
         <v>96</v>
@@ -7146,7 +7148,7 @@
         <v>13</v>
       </c>
       <c r="I167" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="168" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7164,7 +7166,7 @@
         <v>64</v>
       </c>
       <c r="E168" s="47">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F168" s="47" t="s">
         <v>96</v>
@@ -7176,7 +7178,7 @@
         <v>13</v>
       </c>
       <c r="I168" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="169" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7194,7 +7196,7 @@
         <v>64</v>
       </c>
       <c r="E169" s="47">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F169" s="47" t="s">
         <v>96</v>
@@ -7206,7 +7208,7 @@
         <v>13</v>
       </c>
       <c r="I169" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="170" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7224,7 +7226,7 @@
         <v>64</v>
       </c>
       <c r="E170" s="47">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F170" s="47" t="s">
         <v>96</v>
@@ -7236,40 +7238,40 @@
         <v>13</v>
       </c>
       <c r="I170" s="45" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="38">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A171" s="49">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-      <c r="B171" s="38" t="s">
+      <c r="B171" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C171" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D171" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E171" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F171" s="31">
-        <v>1</v>
-      </c>
-      <c r="G171" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="H171" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I171" s="32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D171" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E171" s="47">
+        <v>10</v>
+      </c>
+      <c r="F171" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G171" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H171" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I171" s="45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A172" s="38">
         <f t="shared" si="1"/>
         <v>171</v>
@@ -7280,22 +7282,22 @@
       <c r="C172" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D172" s="6" t="s">
+      <c r="D172" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E172" s="33" t="s">
+      <c r="E172" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="F172" s="25">
-        <v>2</v>
-      </c>
-      <c r="G172" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H172" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I172" s="45" t="s">
+      <c r="F172" s="31">
+        <v>1</v>
+      </c>
+      <c r="G172" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H172" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I172" s="32" t="s">
         <v>105</v>
       </c>
     </row>
@@ -7317,7 +7319,7 @@
         <v>34</v>
       </c>
       <c r="F173" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G173" s="25" t="s">
         <v>96</v>
@@ -7347,7 +7349,7 @@
         <v>34</v>
       </c>
       <c r="F174" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G174" s="25" t="s">
         <v>96</v>
@@ -7377,7 +7379,7 @@
         <v>34</v>
       </c>
       <c r="F175" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G175" s="25" t="s">
         <v>96</v>
@@ -7407,7 +7409,7 @@
         <v>34</v>
       </c>
       <c r="F176" s="25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G176" s="25" t="s">
         <v>96</v>
@@ -7437,7 +7439,7 @@
         <v>34</v>
       </c>
       <c r="F177" s="25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G177" s="25" t="s">
         <v>96</v>
@@ -7467,7 +7469,7 @@
         <v>34</v>
       </c>
       <c r="F178" s="25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G178" s="25" t="s">
         <v>96</v>
@@ -7497,7 +7499,7 @@
         <v>34</v>
       </c>
       <c r="F179" s="25">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G179" s="25" t="s">
         <v>96</v>
@@ -7527,7 +7529,7 @@
         <v>34</v>
       </c>
       <c r="F180" s="25">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G180" s="25" t="s">
         <v>96</v>
@@ -7539,7 +7541,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="181" spans="1:9" s="32" customFormat="1" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="38">
         <f t="shared" si="1"/>
         <v>180</v>
@@ -7550,26 +7552,26 @@
       <c r="C181" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D181" s="30" t="s">
+      <c r="D181" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E181" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F181" s="31">
-        <v>1</v>
-      </c>
-      <c r="G181" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="H181" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I181" s="32" t="s">
+      <c r="E181" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F181" s="25">
+        <v>10</v>
+      </c>
+      <c r="G181" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H181" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I181" s="45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" s="32" customFormat="1" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="38">
         <f t="shared" si="1"/>
         <v>181</v>
@@ -7580,22 +7582,22 @@
       <c r="C182" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D182" s="6" t="s">
+      <c r="D182" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E182" s="34" t="s">
+      <c r="E182" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F182" s="25">
-        <v>2</v>
-      </c>
-      <c r="G182" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H182" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I182" s="45" t="s">
+      <c r="F182" s="31">
+        <v>1</v>
+      </c>
+      <c r="G182" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H182" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I182" s="32" t="s">
         <v>105</v>
       </c>
     </row>
@@ -7617,7 +7619,7 @@
         <v>35</v>
       </c>
       <c r="F183" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G183" s="25" t="s">
         <v>96</v>
@@ -7647,7 +7649,7 @@
         <v>35</v>
       </c>
       <c r="F184" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G184" s="25" t="s">
         <v>96</v>
@@ -7677,7 +7679,7 @@
         <v>35</v>
       </c>
       <c r="F185" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G185" s="25" t="s">
         <v>96</v>
@@ -7707,7 +7709,7 @@
         <v>35</v>
       </c>
       <c r="F186" s="25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G186" s="25" t="s">
         <v>96</v>
@@ -7737,7 +7739,7 @@
         <v>35</v>
       </c>
       <c r="F187" s="25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G187" s="25" t="s">
         <v>96</v>
@@ -7767,7 +7769,7 @@
         <v>35</v>
       </c>
       <c r="F188" s="25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G188" s="25" t="s">
         <v>96</v>
@@ -7797,7 +7799,7 @@
         <v>35</v>
       </c>
       <c r="F189" s="25">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G189" s="25" t="s">
         <v>96</v>
@@ -7827,7 +7829,7 @@
         <v>35</v>
       </c>
       <c r="F190" s="25">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G190" s="25" t="s">
         <v>96</v>
@@ -7839,7 +7841,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="191" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="38">
         <f t="shared" si="1"/>
         <v>190</v>
@@ -7850,52 +7852,52 @@
       <c r="C191" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D191" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="E191" s="29">
-        <v>1</v>
-      </c>
-      <c r="F191" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="G191" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="H191" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I191" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="49">
+      <c r="D191" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E191" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F191" s="25">
+        <v>10</v>
+      </c>
+      <c r="G191" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H191" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I191" s="45" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A192" s="38">
         <f t="shared" si="1"/>
         <v>191</v>
       </c>
-      <c r="B192" s="49" t="s">
+      <c r="B192" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C192" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D192" s="43" t="s">
+      <c r="D192" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="E192" s="47">
+      <c r="E192" s="29">
         <v>1</v>
       </c>
-      <c r="F192" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="G192" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H192" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="I192" s="45" t="s">
+      <c r="F192" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="G192" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H192" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I192" s="32" t="s">
         <v>134</v>
       </c>
     </row>
@@ -7917,7 +7919,7 @@
         <v>1</v>
       </c>
       <c r="F193" s="47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G193" s="47" t="s">
         <v>96</v>
@@ -7947,7 +7949,7 @@
         <v>1</v>
       </c>
       <c r="F194" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G194" s="47" t="s">
         <v>96</v>
@@ -7974,10 +7976,10 @@
         <v>121</v>
       </c>
       <c r="E195" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F195" s="47" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G195" s="47" t="s">
         <v>96</v>
@@ -8007,7 +8009,7 @@
         <v>2</v>
       </c>
       <c r="F196" s="47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G196" s="47" t="s">
         <v>96</v>
@@ -8037,7 +8039,7 @@
         <v>2</v>
       </c>
       <c r="F197" s="47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G197" s="47" t="s">
         <v>96</v>
@@ -8067,7 +8069,7 @@
         <v>2</v>
       </c>
       <c r="F198" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G198" s="47" t="s">
         <v>96</v>
@@ -8094,10 +8096,10 @@
         <v>121</v>
       </c>
       <c r="E199" s="47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F199" s="47" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G199" s="47" t="s">
         <v>96</v>
@@ -8127,7 +8129,7 @@
         <v>3</v>
       </c>
       <c r="F200" s="47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G200" s="47" t="s">
         <v>96</v>
@@ -8157,7 +8159,7 @@
         <v>3</v>
       </c>
       <c r="F201" s="47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G201" s="47" t="s">
         <v>96</v>
@@ -8187,7 +8189,7 @@
         <v>3</v>
       </c>
       <c r="F202" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G202" s="47" t="s">
         <v>96</v>
@@ -8199,41 +8201,67 @@
         <v>134</v>
       </c>
     </row>
-    <row r="203" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="38">
+    <row r="203" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A203" s="49">
         <f t="shared" si="1"/>
         <v>202</v>
       </c>
-      <c r="B203" s="38" t="s">
+      <c r="B203" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C203" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D203" s="30" t="s">
+      <c r="D203" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E203" s="47">
+        <v>3</v>
+      </c>
+      <c r="F203" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G203" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H203" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I203" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A204" s="38">
+        <f t="shared" si="1"/>
+        <v>203</v>
+      </c>
+      <c r="B204" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D204" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E203" s="29" t="s">
+      <c r="E204" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="F203" s="29" t="s">
+      <c r="F204" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="G203" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H203" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I203" s="32" t="s">
+      <c r="G204" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H204" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I204" s="32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D204" s="9"/>
-      <c r="E204" s="9"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D205" s="9"/>
       <c r="E205" s="9"/>
     </row>
@@ -8335,6 +8363,7 @@
     <row r="292" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="293" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="294" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="295" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Added 10 more dropdown-lists in Kombinationsmöglichkeiten
Now there's a total of 20 dropdown-lists in the section Kombinationsmöglichkeiten
</commit_message>
<xml_diff>
--- a/R2Q_Datensatz_leer.xlsx
+++ b/R2Q_Datensatz_leer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pramit\Documents\work\R2Q-Shiny-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8907AFAC-6A8A-4881-864E-770D6CADD401}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D81248-582D-4F11-B237-2729D687885B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E668519-328E-4E8D-8980-09B3972F3278}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="218">
   <si>
     <t>Ressource</t>
   </si>
@@ -657,6 +657,36 @@
   </si>
   <si>
     <t>kosten_hinweis</t>
+  </si>
+  <si>
+    <t>selkombi11</t>
+  </si>
+  <si>
+    <t>selkombi12</t>
+  </si>
+  <si>
+    <t>selkombi13</t>
+  </si>
+  <si>
+    <t>selkombi14</t>
+  </si>
+  <si>
+    <t>selkombi15</t>
+  </si>
+  <si>
+    <t>selkombi16</t>
+  </si>
+  <si>
+    <t>selkombi17</t>
+  </si>
+  <si>
+    <t>selkombi18</t>
+  </si>
+  <si>
+    <t>selkombi19</t>
+  </si>
+  <si>
+    <t>selkombi20</t>
   </si>
 </sst>
 </file>
@@ -1430,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F27926E-B51A-449F-86DD-91CC7FF15C35}">
-  <dimension ref="A1:AA295"/>
+  <dimension ref="A1:AA305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J175" sqref="J175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6793,7 +6823,7 @@
     </row>
     <row r="156" spans="1:27" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="38">
-        <f t="shared" ref="A156:A204" si="1">ROW(A156)-1</f>
+        <f t="shared" ref="A156:A214" si="1">ROW(A156)-1</f>
         <v>155</v>
       </c>
       <c r="B156" s="38" t="s">
@@ -7271,7 +7301,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="172" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A172" s="38">
         <f t="shared" si="1"/>
         <v>171</v>
@@ -7283,295 +7313,295 @@
         <v>96</v>
       </c>
       <c r="D172" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E172" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F172" s="31">
-        <v>1</v>
-      </c>
-      <c r="G172" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E172" s="29">
+        <v>11</v>
+      </c>
+      <c r="F172" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="G172" s="31" t="s">
         <v>96</v>
       </c>
       <c r="H172" s="31" t="s">
         <v>13</v>
       </c>
       <c r="I172" s="32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="38">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A173" s="49">
         <f t="shared" si="1"/>
         <v>172</v>
       </c>
-      <c r="B173" s="38" t="s">
+      <c r="B173" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C173" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D173" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E173" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F173" s="25">
-        <v>2</v>
-      </c>
-      <c r="G173" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H173" s="25" t="s">
+      <c r="D173" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E173" s="47">
+        <v>12</v>
+      </c>
+      <c r="F173" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G173" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H173" s="48" t="s">
         <v>13</v>
       </c>
       <c r="I173" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="38">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A174" s="49">
         <f t="shared" si="1"/>
         <v>173</v>
       </c>
-      <c r="B174" s="38" t="s">
+      <c r="B174" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C174" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D174" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E174" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F174" s="25">
-        <v>3</v>
-      </c>
-      <c r="G174" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H174" s="25" t="s">
+      <c r="D174" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E174" s="47">
+        <v>13</v>
+      </c>
+      <c r="F174" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G174" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H174" s="48" t="s">
         <v>13</v>
       </c>
       <c r="I174" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="38">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A175" s="49">
         <f t="shared" si="1"/>
         <v>174</v>
       </c>
-      <c r="B175" s="38" t="s">
+      <c r="B175" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C175" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D175" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E175" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F175" s="25">
-        <v>4</v>
-      </c>
-      <c r="G175" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H175" s="25" t="s">
+      <c r="D175" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E175" s="47">
+        <v>14</v>
+      </c>
+      <c r="F175" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G175" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H175" s="48" t="s">
         <v>13</v>
       </c>
       <c r="I175" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="38">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A176" s="49">
         <f t="shared" si="1"/>
         <v>175</v>
       </c>
-      <c r="B176" s="38" t="s">
+      <c r="B176" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C176" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D176" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E176" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F176" s="25">
-        <v>5</v>
-      </c>
-      <c r="G176" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H176" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I176" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="38">
+      <c r="D176" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E176" s="47">
+        <v>15</v>
+      </c>
+      <c r="F176" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G176" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H176" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I176" s="32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A177" s="49">
         <f t="shared" si="1"/>
         <v>176</v>
       </c>
-      <c r="B177" s="38" t="s">
+      <c r="B177" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C177" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D177" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E177" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F177" s="25">
-        <v>6</v>
-      </c>
-      <c r="G177" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H177" s="25" t="s">
+      <c r="D177" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E177" s="29">
+        <v>16</v>
+      </c>
+      <c r="F177" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G177" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H177" s="48" t="s">
         <v>13</v>
       </c>
       <c r="I177" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A178" s="38">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A178" s="49">
         <f t="shared" si="1"/>
         <v>177</v>
       </c>
-      <c r="B178" s="38" t="s">
+      <c r="B178" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C178" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D178" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E178" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F178" s="25">
-        <v>7</v>
-      </c>
-      <c r="G178" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H178" s="25" t="s">
+      <c r="D178" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E178" s="47">
+        <v>17</v>
+      </c>
+      <c r="F178" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G178" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H178" s="48" t="s">
         <v>13</v>
       </c>
       <c r="I178" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A179" s="38">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A179" s="49">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
-      <c r="B179" s="38" t="s">
+      <c r="B179" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C179" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D179" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E179" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F179" s="25">
-        <v>8</v>
-      </c>
-      <c r="G179" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H179" s="25" t="s">
+      <c r="D179" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E179" s="47">
+        <v>18</v>
+      </c>
+      <c r="F179" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G179" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H179" s="48" t="s">
         <v>13</v>
       </c>
       <c r="I179" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="38">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A180" s="49">
         <f t="shared" si="1"/>
         <v>179</v>
       </c>
-      <c r="B180" s="38" t="s">
+      <c r="B180" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C180" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D180" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E180" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F180" s="25">
-        <v>9</v>
-      </c>
-      <c r="G180" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H180" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I180" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="38">
+      <c r="D180" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E180" s="47">
+        <v>19</v>
+      </c>
+      <c r="F180" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G180" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H180" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I180" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="49">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="B181" s="38" t="s">
+      <c r="B181" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C181" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D181" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E181" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F181" s="25">
-        <v>10</v>
-      </c>
-      <c r="G181" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H181" s="25" t="s">
+      <c r="D181" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E181" s="47">
+        <v>20</v>
+      </c>
+      <c r="F181" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="G181" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="H181" s="48" t="s">
         <v>13</v>
       </c>
       <c r="I181" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" s="32" customFormat="1" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="38">
         <f t="shared" si="1"/>
         <v>181</v>
@@ -7586,7 +7616,7 @@
         <v>33</v>
       </c>
       <c r="E182" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F182" s="31">
         <v>1</v>
@@ -7615,8 +7645,8 @@
       <c r="D183" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E183" s="34" t="s">
-        <v>35</v>
+      <c r="E183" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F183" s="25">
         <v>2</v>
@@ -7645,8 +7675,8 @@
       <c r="D184" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E184" s="34" t="s">
-        <v>35</v>
+      <c r="E184" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F184" s="25">
         <v>3</v>
@@ -7675,8 +7705,8 @@
       <c r="D185" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E185" s="34" t="s">
-        <v>35</v>
+      <c r="E185" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F185" s="25">
         <v>4</v>
@@ -7705,8 +7735,8 @@
       <c r="D186" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E186" s="34" t="s">
-        <v>35</v>
+      <c r="E186" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F186" s="25">
         <v>5</v>
@@ -7735,8 +7765,8 @@
       <c r="D187" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E187" s="34" t="s">
-        <v>35</v>
+      <c r="E187" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F187" s="25">
         <v>6</v>
@@ -7765,8 +7795,8 @@
       <c r="D188" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E188" s="34" t="s">
-        <v>35</v>
+      <c r="E188" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F188" s="25">
         <v>7</v>
@@ -7795,8 +7825,8 @@
       <c r="D189" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E189" s="34" t="s">
-        <v>35</v>
+      <c r="E189" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F189" s="25">
         <v>8</v>
@@ -7825,8 +7855,8 @@
       <c r="D190" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E190" s="34" t="s">
-        <v>35</v>
+      <c r="E190" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F190" s="25">
         <v>9</v>
@@ -7855,8 +7885,8 @@
       <c r="D191" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E191" s="34" t="s">
-        <v>35</v>
+      <c r="E191" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F191" s="25">
         <v>10</v>
@@ -7871,7 +7901,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="192" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9" s="32" customFormat="1" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A192" s="38">
         <f t="shared" si="1"/>
         <v>191</v>
@@ -7883,14 +7913,14 @@
         <v>96</v>
       </c>
       <c r="D192" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="E192" s="29">
+        <v>33</v>
+      </c>
+      <c r="E192" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F192" s="31">
         <v>1</v>
       </c>
-      <c r="F192" s="29" t="s">
-        <v>135</v>
-      </c>
       <c r="G192" s="29" t="s">
         <v>96</v>
       </c>
@@ -7898,306 +7928,306 @@
         <v>13</v>
       </c>
       <c r="I192" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A193" s="38">
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="B193" s="49" t="s">
+      <c r="B193" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C193" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D193" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E193" s="47">
-        <v>1</v>
-      </c>
-      <c r="F193" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="G193" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H193" s="48" t="s">
+      <c r="D193" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E193" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F193" s="25">
+        <v>2</v>
+      </c>
+      <c r="G193" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H193" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I193" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A194" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A194" s="38">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="B194" s="49" t="s">
+      <c r="B194" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C194" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D194" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E194" s="47">
-        <v>1</v>
-      </c>
-      <c r="F194" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="G194" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H194" s="48" t="s">
+      <c r="D194" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E194" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F194" s="25">
+        <v>3</v>
+      </c>
+      <c r="G194" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H194" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I194" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A195" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A195" s="38">
         <f t="shared" si="1"/>
         <v>194</v>
       </c>
-      <c r="B195" s="49" t="s">
+      <c r="B195" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C195" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D195" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E195" s="47">
-        <v>1</v>
-      </c>
-      <c r="F195" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="G195" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H195" s="48" t="s">
+      <c r="D195" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E195" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F195" s="25">
+        <v>4</v>
+      </c>
+      <c r="G195" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H195" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I195" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A196" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A196" s="38">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
-      <c r="B196" s="49" t="s">
+      <c r="B196" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C196" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D196" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E196" s="47">
-        <v>2</v>
-      </c>
-      <c r="F196" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="G196" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H196" s="48" t="s">
+      <c r="D196" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E196" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F196" s="25">
+        <v>5</v>
+      </c>
+      <c r="G196" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H196" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I196" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A197" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A197" s="38">
         <f t="shared" si="1"/>
         <v>196</v>
       </c>
-      <c r="B197" s="49" t="s">
+      <c r="B197" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C197" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D197" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E197" s="47">
-        <v>2</v>
-      </c>
-      <c r="F197" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="G197" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H197" s="48" t="s">
+      <c r="D197" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E197" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F197" s="25">
+        <v>6</v>
+      </c>
+      <c r="G197" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H197" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I197" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A198" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A198" s="38">
         <f t="shared" si="1"/>
         <v>197</v>
       </c>
-      <c r="B198" s="49" t="s">
+      <c r="B198" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C198" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D198" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E198" s="47">
-        <v>2</v>
-      </c>
-      <c r="F198" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="G198" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H198" s="48" t="s">
+      <c r="D198" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E198" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F198" s="25">
+        <v>7</v>
+      </c>
+      <c r="G198" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H198" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I198" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A199" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A199" s="38">
         <f t="shared" si="1"/>
         <v>198</v>
       </c>
-      <c r="B199" s="49" t="s">
+      <c r="B199" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C199" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D199" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E199" s="47">
-        <v>2</v>
-      </c>
-      <c r="F199" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="G199" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H199" s="48" t="s">
+      <c r="D199" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E199" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F199" s="25">
+        <v>8</v>
+      </c>
+      <c r="G199" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H199" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I199" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A200" s="38">
         <f t="shared" si="1"/>
         <v>199</v>
       </c>
-      <c r="B200" s="49" t="s">
+      <c r="B200" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C200" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D200" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E200" s="47">
-        <v>3</v>
-      </c>
-      <c r="F200" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="G200" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H200" s="48" t="s">
+      <c r="D200" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E200" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F200" s="25">
+        <v>9</v>
+      </c>
+      <c r="G200" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H200" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I200" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A201" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A201" s="38">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="B201" s="49" t="s">
+      <c r="B201" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C201" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D201" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="E201" s="47">
-        <v>3</v>
-      </c>
-      <c r="F201" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="G201" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H201" s="48" t="s">
+      <c r="D201" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E201" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F201" s="25">
+        <v>10</v>
+      </c>
+      <c r="G201" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H201" s="25" t="s">
         <v>13</v>
       </c>
       <c r="I201" s="45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A202" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A202" s="38">
         <f t="shared" si="1"/>
         <v>201</v>
       </c>
-      <c r="B202" s="49" t="s">
+      <c r="B202" s="38" t="s">
         <v>98</v>
       </c>
       <c r="C202" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D202" s="43" t="s">
+      <c r="D202" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="E202" s="47">
-        <v>3</v>
-      </c>
-      <c r="F202" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="G202" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H202" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="I202" s="45" t="s">
+      <c r="E202" s="29">
+        <v>1</v>
+      </c>
+      <c r="F202" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="G202" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H202" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I202" s="32" t="s">
         <v>134</v>
       </c>
     </row>
@@ -8216,10 +8246,10 @@
         <v>121</v>
       </c>
       <c r="E203" s="47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F203" s="47" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G203" s="47" t="s">
         <v>96</v>
@@ -8231,139 +8261,700 @@
         <v>134</v>
       </c>
     </row>
-    <row r="204" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="38">
+    <row r="204" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A204" s="49">
         <f t="shared" si="1"/>
         <v>203</v>
       </c>
-      <c r="B204" s="38" t="s">
+      <c r="B204" s="49" t="s">
         <v>98</v>
       </c>
       <c r="C204" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D204" s="30" t="s">
+      <c r="D204" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E204" s="47">
+        <v>1</v>
+      </c>
+      <c r="F204" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="G204" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H204" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I204" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A205" s="49">
+        <f t="shared" si="1"/>
+        <v>204</v>
+      </c>
+      <c r="B205" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D205" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E205" s="47">
+        <v>1</v>
+      </c>
+      <c r="F205" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G205" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H205" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I205" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A206" s="49">
+        <f t="shared" si="1"/>
+        <v>205</v>
+      </c>
+      <c r="B206" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D206" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E206" s="47">
+        <v>2</v>
+      </c>
+      <c r="F206" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G206" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H206" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I206" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A207" s="49">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="B207" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C207" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D207" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E207" s="47">
+        <v>2</v>
+      </c>
+      <c r="F207" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="G207" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H207" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I207" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A208" s="49">
+        <f t="shared" si="1"/>
+        <v>207</v>
+      </c>
+      <c r="B208" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C208" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D208" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E208" s="47">
+        <v>2</v>
+      </c>
+      <c r="F208" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="G208" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H208" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I208" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A209" s="49">
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+      <c r="B209" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C209" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D209" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E209" s="47">
+        <v>2</v>
+      </c>
+      <c r="F209" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G209" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H209" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I209" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A210" s="49">
+        <f t="shared" si="1"/>
+        <v>209</v>
+      </c>
+      <c r="B210" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C210" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D210" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E210" s="47">
+        <v>3</v>
+      </c>
+      <c r="F210" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G210" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H210" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I210" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A211" s="49">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="B211" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C211" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D211" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E211" s="47">
+        <v>3</v>
+      </c>
+      <c r="F211" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="G211" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H211" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I211" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A212" s="49">
+        <f t="shared" si="1"/>
+        <v>211</v>
+      </c>
+      <c r="B212" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C212" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D212" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E212" s="47">
+        <v>3</v>
+      </c>
+      <c r="F212" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="G212" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H212" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I212" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" s="45" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A213" s="49">
+        <f t="shared" si="1"/>
+        <v>212</v>
+      </c>
+      <c r="B213" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C213" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D213" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E213" s="47">
+        <v>3</v>
+      </c>
+      <c r="F213" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G213" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H213" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I213" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" s="32" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A214" s="38">
+        <f t="shared" si="1"/>
+        <v>213</v>
+      </c>
+      <c r="B214" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C214" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D214" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E204" s="29" t="s">
+      <c r="E214" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="F204" s="29" t="s">
+      <c r="F214" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="G204" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="H204" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I204" s="32" t="s">
+      <c r="G214" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H214" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I214" s="32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D205" s="9"/>
-      <c r="E205" s="9"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D206" s="9"/>
-      <c r="E206" s="9"/>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D207" s="9"/>
-      <c r="E207" s="9"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D208" s="9"/>
-      <c r="E208" s="9"/>
-    </row>
-    <row r="209" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="210" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="211" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="212" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="213" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="214" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="215" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="216" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="217" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="218" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="219" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="220" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="221" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="222" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="223" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="224" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="225" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="226" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="227" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="228" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="229" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="230" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="231" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="232" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="233" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="234" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="235" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="236" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="237" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="238" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="239" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="240" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="241" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="242" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="243" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="244" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="245" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="246" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="247" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="248" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="249" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="250" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="251" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="252" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="253" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="254" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="255" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="256" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="257" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="258" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="259" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="260" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="261" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="262" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="263" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="264" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="265" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="266" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="267" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="268" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="269" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="270" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="271" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="272" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="273" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="274" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="275" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="276" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="277" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="278" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="279" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="280" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="281" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="282" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="283" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="284" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="285" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="286" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="287" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="288" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="289" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="290" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="291" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="292" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="293" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="294" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="295" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="215" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D215" s="9"/>
+      <c r="E215" s="9"/>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D216" s="9"/>
+      <c r="E216" s="9"/>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D217" s="9"/>
+      <c r="E217" s="9"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D218" s="9"/>
+      <c r="E218" s="9"/>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D219" s="9"/>
+      <c r="E219" s="9"/>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D220" s="9"/>
+      <c r="E220" s="9"/>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D221" s="9"/>
+      <c r="E221" s="9"/>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D222" s="9"/>
+      <c r="E222" s="9"/>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D223" s="9"/>
+      <c r="E223" s="9"/>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D224" s="9"/>
+      <c r="E224" s="9"/>
+    </row>
+    <row r="225" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D225" s="9"/>
+      <c r="E225" s="9"/>
+    </row>
+    <row r="226" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D226" s="9"/>
+      <c r="E226" s="9"/>
+    </row>
+    <row r="227" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D227" s="9"/>
+      <c r="E227" s="9"/>
+    </row>
+    <row r="228" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D228" s="9"/>
+      <c r="E228" s="9"/>
+    </row>
+    <row r="229" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D229" s="9"/>
+      <c r="E229" s="9"/>
+    </row>
+    <row r="230" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D230" s="9"/>
+      <c r="E230" s="9"/>
+    </row>
+    <row r="231" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D231" s="9"/>
+      <c r="E231" s="9"/>
+    </row>
+    <row r="232" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D232" s="9"/>
+      <c r="E232" s="9"/>
+    </row>
+    <row r="233" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D233" s="9"/>
+      <c r="E233" s="9"/>
+    </row>
+    <row r="234" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D234" s="9"/>
+      <c r="E234" s="9"/>
+    </row>
+    <row r="235" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D235" s="9"/>
+      <c r="E235" s="9"/>
+    </row>
+    <row r="236" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D236" s="9"/>
+      <c r="E236" s="9"/>
+    </row>
+    <row r="237" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D237" s="9"/>
+      <c r="E237" s="9"/>
+    </row>
+    <row r="238" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D238" s="9"/>
+      <c r="E238" s="9"/>
+    </row>
+    <row r="239" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D239" s="9"/>
+      <c r="E239" s="9"/>
+    </row>
+    <row r="240" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D240" s="9"/>
+      <c r="E240" s="9"/>
+    </row>
+    <row r="241" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D241" s="9"/>
+      <c r="E241" s="9"/>
+    </row>
+    <row r="242" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D242" s="9"/>
+      <c r="E242" s="9"/>
+    </row>
+    <row r="243" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D243" s="9"/>
+      <c r="E243" s="9"/>
+    </row>
+    <row r="244" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D244" s="9"/>
+      <c r="E244" s="9"/>
+    </row>
+    <row r="245" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D245" s="9"/>
+      <c r="E245" s="9"/>
+    </row>
+    <row r="246" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D246" s="9"/>
+      <c r="E246" s="9"/>
+    </row>
+    <row r="247" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D247" s="9"/>
+      <c r="E247" s="9"/>
+    </row>
+    <row r="248" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D248" s="9"/>
+      <c r="E248" s="9"/>
+    </row>
+    <row r="249" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D249" s="9"/>
+      <c r="E249" s="9"/>
+    </row>
+    <row r="250" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D250" s="9"/>
+      <c r="E250" s="9"/>
+    </row>
+    <row r="251" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D251" s="9"/>
+      <c r="E251" s="9"/>
+    </row>
+    <row r="252" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D252" s="9"/>
+      <c r="E252" s="9"/>
+    </row>
+    <row r="253" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D253" s="9"/>
+      <c r="E253" s="9"/>
+    </row>
+    <row r="254" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D254" s="9"/>
+      <c r="E254" s="9"/>
+    </row>
+    <row r="255" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D255" s="9"/>
+      <c r="E255" s="9"/>
+    </row>
+    <row r="256" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D256" s="9"/>
+      <c r="E256" s="9"/>
+    </row>
+    <row r="257" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D257" s="9"/>
+      <c r="E257" s="9"/>
+    </row>
+    <row r="258" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D258" s="9"/>
+      <c r="E258" s="9"/>
+    </row>
+    <row r="259" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D259" s="9"/>
+      <c r="E259" s="9"/>
+    </row>
+    <row r="260" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D260" s="9"/>
+      <c r="E260" s="9"/>
+    </row>
+    <row r="261" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D261" s="9"/>
+      <c r="E261" s="9"/>
+    </row>
+    <row r="262" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D262" s="9"/>
+      <c r="E262" s="9"/>
+    </row>
+    <row r="263" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D263" s="9"/>
+      <c r="E263" s="9"/>
+    </row>
+    <row r="264" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D264" s="9"/>
+      <c r="E264" s="9"/>
+    </row>
+    <row r="265" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D265" s="9"/>
+      <c r="E265" s="9"/>
+    </row>
+    <row r="266" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D266" s="9"/>
+      <c r="E266" s="9"/>
+    </row>
+    <row r="267" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D267" s="9"/>
+      <c r="E267" s="9"/>
+    </row>
+    <row r="268" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D268" s="9"/>
+      <c r="E268" s="9"/>
+    </row>
+    <row r="269" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D269" s="9"/>
+      <c r="E269" s="9"/>
+    </row>
+    <row r="270" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D270" s="9"/>
+      <c r="E270" s="9"/>
+    </row>
+    <row r="271" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D271" s="9"/>
+      <c r="E271" s="9"/>
+    </row>
+    <row r="272" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D272" s="9"/>
+      <c r="E272" s="9"/>
+    </row>
+    <row r="273" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D273" s="9"/>
+      <c r="E273" s="9"/>
+    </row>
+    <row r="274" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D274" s="9"/>
+      <c r="E274" s="9"/>
+    </row>
+    <row r="275" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D275" s="9"/>
+      <c r="E275" s="9"/>
+    </row>
+    <row r="276" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D276" s="9"/>
+      <c r="E276" s="9"/>
+    </row>
+    <row r="277" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D277" s="9"/>
+      <c r="E277" s="9"/>
+    </row>
+    <row r="278" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D278" s="9"/>
+      <c r="E278" s="9"/>
+    </row>
+    <row r="279" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D279" s="9"/>
+      <c r="E279" s="9"/>
+    </row>
+    <row r="280" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D280" s="9"/>
+      <c r="E280" s="9"/>
+    </row>
+    <row r="281" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D281" s="9"/>
+      <c r="E281" s="9"/>
+    </row>
+    <row r="282" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D282" s="9"/>
+      <c r="E282" s="9"/>
+    </row>
+    <row r="283" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D283" s="9"/>
+      <c r="E283" s="9"/>
+    </row>
+    <row r="284" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D284" s="9"/>
+      <c r="E284" s="9"/>
+    </row>
+    <row r="285" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D285" s="9"/>
+      <c r="E285" s="9"/>
+    </row>
+    <row r="286" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D286" s="9"/>
+      <c r="E286" s="9"/>
+    </row>
+    <row r="287" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D287" s="9"/>
+      <c r="E287" s="9"/>
+    </row>
+    <row r="288" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D288" s="9"/>
+      <c r="E288" s="9"/>
+    </row>
+    <row r="289" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D289" s="9"/>
+      <c r="E289" s="9"/>
+    </row>
+    <row r="290" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D290" s="9"/>
+      <c r="E290" s="9"/>
+    </row>
+    <row r="291" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D291" s="9"/>
+      <c r="E291" s="9"/>
+    </row>
+    <row r="292" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D292" s="9"/>
+      <c r="E292" s="9"/>
+    </row>
+    <row r="293" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D293" s="9"/>
+      <c r="E293" s="9"/>
+    </row>
+    <row r="294" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D294" s="9"/>
+      <c r="E294" s="9"/>
+    </row>
+    <row r="295" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D295" s="9"/>
+      <c r="E295" s="9"/>
+    </row>
+    <row r="296" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D296" s="9"/>
+      <c r="E296" s="9"/>
+    </row>
+    <row r="297" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D297" s="9"/>
+      <c r="E297" s="9"/>
+    </row>
+    <row r="298" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D298" s="9"/>
+      <c r="E298" s="9"/>
+    </row>
+    <row r="299" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D299" s="9"/>
+      <c r="E299" s="9"/>
+    </row>
+    <row r="300" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D300" s="9"/>
+      <c r="E300" s="9"/>
+    </row>
+    <row r="301" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D301" s="9"/>
+      <c r="E301" s="9"/>
+    </row>
+    <row r="302" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D302" s="9"/>
+      <c r="E302" s="9"/>
+    </row>
+    <row r="303" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D303" s="9"/>
+      <c r="E303" s="9"/>
+    </row>
+    <row r="304" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D304" s="9"/>
+      <c r="E304" s="9"/>
+    </row>
+    <row r="305" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D305" s="9"/>
+      <c r="E305" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
box names updated in spreadsheet
</commit_message>
<xml_diff>
--- a/R2Q_Datensatz_leer.xlsx
+++ b/R2Q_Datensatz_leer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="238">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -169,61 +169,103 @@
     <t xml:space="preserve">Vermeidung</t>
   </si>
   <si>
-    <t xml:space="preserve">cbgbaustoffe</t>
+    <t xml:space="preserve">baustoffe_1</t>
   </si>
   <si>
     <t xml:space="preserve">Wiederverwendung</t>
   </si>
   <si>
+    <t xml:space="preserve">baustoffe_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recycling</t>
   </si>
   <si>
+    <t xml:space="preserve">baustoffe_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Verwertung</t>
   </si>
   <si>
+    <t xml:space="preserve">baustoffe_4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beseitigung</t>
   </si>
   <si>
+    <t xml:space="preserve">baustoffe_5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Klimaanpassung</t>
   </si>
   <si>
-    <t xml:space="preserve">cbgflaeche</t>
+    <t xml:space="preserve">flaeche_1</t>
   </si>
   <si>
     <t xml:space="preserve">Gesundheitsschutz</t>
   </si>
   <si>
+    <t xml:space="preserve">flaeche_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Erhalt d. Grunddaseinsfunktion</t>
   </si>
   <si>
+    <t xml:space="preserve">flaeche_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Naturschutz</t>
   </si>
   <si>
+    <t xml:space="preserve">flaeche_4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Klimaschutz</t>
   </si>
   <si>
+    <t xml:space="preserve">flaeche_5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Energiebereitstellung</t>
   </si>
   <si>
-    <t xml:space="preserve">cbgenergie</t>
+    <t xml:space="preserve">energie_1</t>
   </si>
   <si>
     <t xml:space="preserve">Energieverteilung</t>
   </si>
   <si>
+    <t xml:space="preserve">energie_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Energieverbrauch</t>
   </si>
   <si>
+    <t xml:space="preserve">energie_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Energiespeicherung</t>
   </si>
   <si>
+    <t xml:space="preserve">energie_4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elektrizität</t>
   </si>
   <si>
+    <t xml:space="preserve">energie_5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wärme</t>
   </si>
   <si>
+    <t xml:space="preserve">energie_6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brennstoffe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energie_7</t>
   </si>
   <si>
     <t xml:space="preserve">Anwendungsebene</t>
@@ -1273,11 +1315,11 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.87890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.11"/>
@@ -1915,7 +1957,7 @@
         <v>24</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,7 +1978,7 @@
         <v>27</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G22" s="24" t="s">
         <v>8</v>
@@ -1945,7 +1987,7 @@
         <v>24</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,7 +2008,7 @@
         <v>27</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>8</v>
@@ -1975,7 +2017,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1996,7 +2038,7 @@
         <v>27</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G24" s="24" t="s">
         <v>8</v>
@@ -2005,7 +2047,7 @@
         <v>24</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,7 +2068,7 @@
         <v>29</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G25" s="33" t="s">
         <v>8</v>
@@ -2035,7 +2077,7 @@
         <v>24</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,7 +2098,7 @@
         <v>29</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>8</v>
@@ -2065,7 +2107,7 @@
         <v>24</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,7 +2128,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G27" s="24" t="s">
         <v>8</v>
@@ -2095,7 +2137,7 @@
         <v>24</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,7 +2158,7 @@
         <v>29</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G28" s="24" t="s">
         <v>8</v>
@@ -2125,7 +2167,7 @@
         <v>24</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,7 +2188,7 @@
         <v>29</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G29" s="24" t="s">
         <v>8</v>
@@ -2155,7 +2197,7 @@
         <v>24</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,7 +2218,7 @@
         <v>28</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G30" s="24" t="s">
         <v>8</v>
@@ -2185,7 +2227,7 @@
         <v>24</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2206,7 +2248,7 @@
         <v>28</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>8</v>
@@ -2215,7 +2257,7 @@
         <v>24</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2236,7 +2278,7 @@
         <v>28</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G32" s="24" t="s">
         <v>8</v>
@@ -2245,7 +2287,7 @@
         <v>24</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2266,7 +2308,7 @@
         <v>28</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G33" s="24" t="s">
         <v>8</v>
@@ -2275,7 +2317,7 @@
         <v>24</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,7 +2338,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="G34" s="24" t="s">
         <v>8</v>
@@ -2305,7 +2347,7 @@
         <v>24</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2326,7 +2368,7 @@
         <v>28</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="G35" s="24" t="s">
         <v>8</v>
@@ -2335,7 +2377,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2355,7 +2397,7 @@
         <v>28</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="G36" s="24" t="s">
         <v>8</v>
@@ -2364,7 +2406,7 @@
         <v>24</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,10 +2421,10 @@
         <v>8</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F37" s="30" t="s">
         <v>8</v>
@@ -2394,7 +2436,7 @@
         <v>24</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,10 +2451,10 @@
         <v>8</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E38" s="35" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="F38" s="24" t="s">
         <v>8</v>
@@ -2424,7 +2466,7 @@
         <v>24</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2439,10 +2481,10 @@
         <v>8</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="F39" s="24" t="s">
         <v>8</v>
@@ -2454,7 +2496,7 @@
         <v>24</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,10 +2511,10 @@
         <v>8</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="F40" s="30" t="s">
         <v>8</v>
@@ -2481,10 +2523,10 @@
         <v>8</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2499,10 +2541,10 @@
         <v>8</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F41" s="37" t="s">
         <v>8</v>
@@ -2511,10 +2553,10 @@
         <v>8</v>
       </c>
       <c r="H41" s="37" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="I41" s="38" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2529,10 +2571,10 @@
         <v>8</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="F42" s="37" t="s">
         <v>8</v>
@@ -2541,10 +2583,10 @@
         <v>8</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2559,10 +2601,10 @@
         <v>8</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="F43" s="30" t="s">
         <v>8</v>
@@ -2571,10 +2613,10 @@
         <v>8</v>
       </c>
       <c r="H43" s="30" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,10 +2631,10 @@
         <v>8</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E44" s="40" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="F44" s="37" t="s">
         <v>8</v>
@@ -2601,10 +2643,10 @@
         <v>8</v>
       </c>
       <c r="H44" s="37" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,10 +2661,10 @@
         <v>8</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E45" s="40" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="F45" s="37" t="s">
         <v>8</v>
@@ -2631,10 +2673,10 @@
         <v>8</v>
       </c>
       <c r="H45" s="37" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" s="16" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2649,10 +2691,10 @@
         <v>8</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="F46" s="30" t="s">
         <v>8</v>
@@ -2664,7 +2706,7 @@
         <v>24</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2679,10 +2721,10 @@
         <v>8</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E47" s="41" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="F47" s="37" t="s">
         <v>8</v>
@@ -2694,7 +2736,7 @@
         <v>24</v>
       </c>
       <c r="I47" s="38" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,10 +2751,10 @@
         <v>8</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E48" s="41" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="F48" s="37" t="s">
         <v>8</v>
@@ -2724,7 +2766,7 @@
         <v>24</v>
       </c>
       <c r="I48" s="38" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2739,10 +2781,10 @@
         <v>8</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="E49" s="41" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F49" s="37" t="s">
         <v>8</v>
@@ -2754,7 +2796,7 @@
         <v>13</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2769,7 +2811,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E50" s="29" t="s">
         <v>8</v>
@@ -2784,7 +2826,7 @@
         <v>13</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2799,7 +2841,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>16</v>
@@ -2814,7 +2856,7 @@
         <v>17</v>
       </c>
       <c r="I51" s="16" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,7 +2871,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="E52" s="29" t="s">
         <v>19</v>
@@ -2844,7 +2886,7 @@
         <v>13</v>
       </c>
       <c r="I52" s="16" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,7 +2901,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="E53" s="29" t="s">
         <v>21</v>
@@ -2874,7 +2916,7 @@
         <v>13</v>
       </c>
       <c r="I53" s="16" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" s="16" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2889,10 +2931,10 @@
         <v>8</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="F54" s="30" t="s">
         <v>8</v>
@@ -2904,7 +2946,7 @@
         <v>13</v>
       </c>
       <c r="I54" s="16" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2919,10 +2961,10 @@
         <v>8</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E55" s="42" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="F55" s="43" t="s">
         <v>8</v>
@@ -2934,7 +2976,7 @@
         <v>13</v>
       </c>
       <c r="I55" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2949,10 +2991,10 @@
         <v>8</v>
       </c>
       <c r="D56" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E56" s="42" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="F56" s="43" t="s">
         <v>8</v>
@@ -2964,7 +3006,7 @@
         <v>13</v>
       </c>
       <c r="I56" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2979,10 +3021,10 @@
         <v>8</v>
       </c>
       <c r="D57" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E57" s="42" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="F57" s="43" t="s">
         <v>8</v>
@@ -2994,7 +3036,7 @@
         <v>13</v>
       </c>
       <c r="I57" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3009,10 +3051,10 @@
         <v>8</v>
       </c>
       <c r="D58" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E58" s="42" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="F58" s="43" t="s">
         <v>8</v>
@@ -3024,7 +3066,7 @@
         <v>13</v>
       </c>
       <c r="I58" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3039,10 +3081,10 @@
         <v>8</v>
       </c>
       <c r="D59" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E59" s="42" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="F59" s="43" t="s">
         <v>8</v>
@@ -3054,7 +3096,7 @@
         <v>13</v>
       </c>
       <c r="I59" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,10 +3111,10 @@
         <v>8</v>
       </c>
       <c r="D60" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E60" s="42" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="F60" s="43" t="s">
         <v>8</v>
@@ -3084,7 +3126,7 @@
         <v>13</v>
       </c>
       <c r="I60" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3099,10 +3141,10 @@
         <v>8</v>
       </c>
       <c r="D61" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E61" s="42" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="F61" s="43" t="s">
         <v>8</v>
@@ -3114,7 +3156,7 @@
         <v>13</v>
       </c>
       <c r="I61" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3129,10 +3171,10 @@
         <v>8</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E62" s="42" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="F62" s="43" t="s">
         <v>8</v>
@@ -3144,7 +3186,7 @@
         <v>13</v>
       </c>
       <c r="I62" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,10 +3201,10 @@
         <v>8</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E63" s="42" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="F63" s="43" t="s">
         <v>8</v>
@@ -3174,7 +3216,7 @@
         <v>13</v>
       </c>
       <c r="I63" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" s="38" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3189,10 +3231,10 @@
         <v>8</v>
       </c>
       <c r="D64" s="42" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E64" s="42" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="F64" s="43" t="s">
         <v>8</v>
@@ -3204,7 +3246,7 @@
         <v>13</v>
       </c>
       <c r="I64" s="38" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,10 +3261,10 @@
         <v>8</v>
       </c>
       <c r="D65" s="29" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="F65" s="30" t="s">
         <v>8</v>
@@ -3234,7 +3276,7 @@
         <v>13</v>
       </c>
       <c r="I65" s="16" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3249,13 +3291,13 @@
         <v>8</v>
       </c>
       <c r="D66" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E66" s="42" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="F66" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G66" s="43" t="s">
         <v>8</v>
@@ -3264,7 +3306,7 @@
         <v>13</v>
       </c>
       <c r="I66" s="44" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3279,13 +3321,13 @@
         <v>8</v>
       </c>
       <c r="D67" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E67" s="42" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="F67" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G67" s="43" t="s">
         <v>8</v>
@@ -3294,7 +3336,7 @@
         <v>13</v>
       </c>
       <c r="I67" s="44" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3309,13 +3351,13 @@
         <v>8</v>
       </c>
       <c r="D68" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E68" s="42" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="F68" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G68" s="43" t="s">
         <v>8</v>
@@ -3324,7 +3366,7 @@
         <v>13</v>
       </c>
       <c r="I68" s="44" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3339,13 +3381,13 @@
         <v>8</v>
       </c>
       <c r="D69" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E69" s="42" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="F69" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G69" s="43" t="s">
         <v>8</v>
@@ -3354,7 +3396,7 @@
         <v>13</v>
       </c>
       <c r="I69" s="44" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3369,13 +3411,13 @@
         <v>8</v>
       </c>
       <c r="D70" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E70" s="42" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="F70" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G70" s="43" t="s">
         <v>8</v>
@@ -3384,7 +3426,7 @@
         <v>13</v>
       </c>
       <c r="I70" s="44" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3399,13 +3441,13 @@
         <v>8</v>
       </c>
       <c r="D71" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E71" s="42" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="F71" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G71" s="43" t="s">
         <v>8</v>
@@ -3414,7 +3456,7 @@
         <v>13</v>
       </c>
       <c r="I71" s="44" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,13 +3471,13 @@
         <v>8</v>
       </c>
       <c r="D72" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E72" s="42" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="F72" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G72" s="43" t="s">
         <v>8</v>
@@ -3444,7 +3486,7 @@
         <v>13</v>
       </c>
       <c r="I72" s="44" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,13 +3501,13 @@
         <v>8</v>
       </c>
       <c r="D73" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E73" s="42" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="F73" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G73" s="43" t="s">
         <v>8</v>
@@ -3474,7 +3516,7 @@
         <v>13</v>
       </c>
       <c r="I73" s="44" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3489,13 +3531,13 @@
         <v>8</v>
       </c>
       <c r="D74" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E74" s="42" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="F74" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G74" s="43" t="s">
         <v>8</v>
@@ -3504,7 +3546,7 @@
         <v>13</v>
       </c>
       <c r="I74" s="44" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,13 +3561,13 @@
         <v>8</v>
       </c>
       <c r="D75" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E75" s="42" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="F75" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G75" s="43" t="s">
         <v>8</v>
@@ -3534,7 +3576,7 @@
         <v>13</v>
       </c>
       <c r="I75" s="44" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3549,13 +3591,13 @@
         <v>8</v>
       </c>
       <c r="D76" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E76" s="42" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="F76" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G76" s="43" t="s">
         <v>8</v>
@@ -3564,7 +3606,7 @@
         <v>13</v>
       </c>
       <c r="I76" s="44" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3579,13 +3621,13 @@
         <v>8</v>
       </c>
       <c r="D77" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E77" s="42" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="F77" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G77" s="43" t="s">
         <v>8</v>
@@ -3594,7 +3636,7 @@
         <v>13</v>
       </c>
       <c r="I77" s="44" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3609,13 +3651,13 @@
         <v>8</v>
       </c>
       <c r="D78" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E78" s="42" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="F78" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G78" s="43" t="s">
         <v>8</v>
@@ -3624,7 +3666,7 @@
         <v>13</v>
       </c>
       <c r="I78" s="44" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3639,13 +3681,13 @@
         <v>8</v>
       </c>
       <c r="D79" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E79" s="42" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="F79" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G79" s="43" t="s">
         <v>8</v>
@@ -3654,7 +3696,7 @@
         <v>13</v>
       </c>
       <c r="I79" s="44" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3669,13 +3711,13 @@
         <v>8</v>
       </c>
       <c r="D80" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E80" s="42" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="F80" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G80" s="43" t="s">
         <v>8</v>
@@ -3684,7 +3726,7 @@
         <v>13</v>
       </c>
       <c r="I80" s="44" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,13 +3741,13 @@
         <v>8</v>
       </c>
       <c r="D81" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E81" s="42" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="F81" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G81" s="43" t="s">
         <v>8</v>
@@ -3714,7 +3756,7 @@
         <v>13</v>
       </c>
       <c r="I81" s="44" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3729,13 +3771,13 @@
         <v>8</v>
       </c>
       <c r="D82" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E82" s="42" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="F82" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G82" s="43" t="s">
         <v>8</v>
@@ -3744,7 +3786,7 @@
         <v>13</v>
       </c>
       <c r="I82" s="44" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3759,13 +3801,13 @@
         <v>8</v>
       </c>
       <c r="D83" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E83" s="42" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="F83" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G83" s="43" t="s">
         <v>8</v>
@@ -3774,7 +3816,7 @@
         <v>13</v>
       </c>
       <c r="I83" s="44" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3789,13 +3831,13 @@
         <v>8</v>
       </c>
       <c r="D84" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E84" s="42" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="F84" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G84" s="43" t="s">
         <v>8</v>
@@ -3804,7 +3846,7 @@
         <v>13</v>
       </c>
       <c r="I84" s="44" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
     <row r="85" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3819,13 +3861,13 @@
         <v>8</v>
       </c>
       <c r="D85" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E85" s="42" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="F85" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G85" s="43" t="s">
         <v>8</v>
@@ -3834,7 +3876,7 @@
         <v>13</v>
       </c>
       <c r="I85" s="44" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3849,13 +3891,13 @@
         <v>8</v>
       </c>
       <c r="D86" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E86" s="42" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F86" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G86" s="43" t="s">
         <v>8</v>
@@ -3864,7 +3906,7 @@
         <v>13</v>
       </c>
       <c r="I86" s="44" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3879,13 +3921,13 @@
         <v>8</v>
       </c>
       <c r="D87" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E87" s="42" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F87" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G87" s="43" t="s">
         <v>8</v>
@@ -3894,7 +3936,7 @@
         <v>13</v>
       </c>
       <c r="I87" s="44" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3909,13 +3951,13 @@
         <v>8</v>
       </c>
       <c r="D88" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E88" s="42" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F88" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G88" s="43" t="s">
         <v>8</v>
@@ -3924,7 +3966,7 @@
         <v>13</v>
       </c>
       <c r="I88" s="44" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3939,13 +3981,13 @@
         <v>8</v>
       </c>
       <c r="D89" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E89" s="42" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F89" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G89" s="43" t="s">
         <v>8</v>
@@ -3954,7 +3996,7 @@
         <v>13</v>
       </c>
       <c r="I89" s="44" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3969,13 +4011,13 @@
         <v>8</v>
       </c>
       <c r="D90" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E90" s="42" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="F90" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G90" s="43" t="s">
         <v>8</v>
@@ -3984,7 +4026,7 @@
         <v>13</v>
       </c>
       <c r="I90" s="44" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,13 +4041,13 @@
         <v>8</v>
       </c>
       <c r="D91" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E91" s="42" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="F91" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G91" s="43" t="s">
         <v>8</v>
@@ -4014,7 +4056,7 @@
         <v>13</v>
       </c>
       <c r="I91" s="44" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4029,13 +4071,13 @@
         <v>8</v>
       </c>
       <c r="D92" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E92" s="42" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="F92" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G92" s="43" t="s">
         <v>8</v>
@@ -4044,7 +4086,7 @@
         <v>13</v>
       </c>
       <c r="I92" s="44" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4059,13 +4101,13 @@
         <v>8</v>
       </c>
       <c r="D93" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E93" s="42" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="F93" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G93" s="43" t="s">
         <v>8</v>
@@ -4074,7 +4116,7 @@
         <v>13</v>
       </c>
       <c r="I93" s="44" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4089,13 +4131,13 @@
         <v>8</v>
       </c>
       <c r="D94" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E94" s="42" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="F94" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G94" s="43" t="s">
         <v>8</v>
@@ -4104,7 +4146,7 @@
         <v>13</v>
       </c>
       <c r="I94" s="44" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="95" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4119,13 +4161,13 @@
         <v>8</v>
       </c>
       <c r="D95" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E95" s="42" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="F95" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G95" s="43" t="s">
         <v>8</v>
@@ -4134,7 +4176,7 @@
         <v>13</v>
       </c>
       <c r="I95" s="44" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4149,13 +4191,13 @@
         <v>8</v>
       </c>
       <c r="D96" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E96" s="42" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="F96" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G96" s="43" t="s">
         <v>8</v>
@@ -4164,7 +4206,7 @@
         <v>13</v>
       </c>
       <c r="I96" s="44" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="97" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4179,13 +4221,13 @@
         <v>8</v>
       </c>
       <c r="D97" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E97" s="42" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="F97" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G97" s="43" t="s">
         <v>8</v>
@@ -4194,7 +4236,7 @@
         <v>13</v>
       </c>
       <c r="I97" s="44" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,13 +4251,13 @@
         <v>8</v>
       </c>
       <c r="D98" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E98" s="42" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="F98" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G98" s="43" t="s">
         <v>8</v>
@@ -4224,7 +4266,7 @@
         <v>13</v>
       </c>
       <c r="I98" s="44" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="99" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4239,13 +4281,13 @@
         <v>8</v>
       </c>
       <c r="D99" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E99" s="42" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="F99" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G99" s="43" t="s">
         <v>8</v>
@@ -4254,7 +4296,7 @@
         <v>13</v>
       </c>
       <c r="I99" s="44" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="100" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4269,13 +4311,13 @@
         <v>8</v>
       </c>
       <c r="D100" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E100" s="42" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="F100" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G100" s="43" t="s">
         <v>8</v>
@@ -4284,7 +4326,7 @@
         <v>13</v>
       </c>
       <c r="I100" s="44" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
     </row>
     <row r="101" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4299,13 +4341,13 @@
         <v>8</v>
       </c>
       <c r="D101" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E101" s="42" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="F101" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G101" s="43" t="s">
         <v>8</v>
@@ -4314,7 +4356,7 @@
         <v>13</v>
       </c>
       <c r="I101" s="44" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="102" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4329,13 +4371,13 @@
         <v>8</v>
       </c>
       <c r="D102" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E102" s="42" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="F102" s="43" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G102" s="43" t="s">
         <v>8</v>
@@ -4344,7 +4386,7 @@
         <v>13</v>
       </c>
       <c r="I102" s="44" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
     </row>
     <row r="103" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4359,13 +4401,13 @@
         <v>8</v>
       </c>
       <c r="D103" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E103" s="42" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="F103" s="43" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G103" s="43" t="s">
         <v>8</v>
@@ -4374,7 +4416,7 @@
         <v>13</v>
       </c>
       <c r="I103" s="44" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4389,13 +4431,13 @@
         <v>8</v>
       </c>
       <c r="D104" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E104" s="42" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="F104" s="43" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G104" s="43" t="s">
         <v>8</v>
@@ -4404,7 +4446,7 @@
         <v>13</v>
       </c>
       <c r="I104" s="44" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4419,13 +4461,13 @@
         <v>8</v>
       </c>
       <c r="D105" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E105" s="42" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="F105" s="43" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="G105" s="43" t="s">
         <v>8</v>
@@ -4434,7 +4476,7 @@
         <v>13</v>
       </c>
       <c r="I105" s="44" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="106" s="38" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4448,10 +4490,10 @@
         <v>8</v>
       </c>
       <c r="D106" s="42" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E106" s="42" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F106" s="43" t="s">
         <v>8</v>
@@ -4463,7 +4505,7 @@
         <v>13</v>
       </c>
       <c r="I106" s="44" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="107" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4478,10 +4520,10 @@
         <v>8</v>
       </c>
       <c r="D107" s="45" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E107" s="45" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>8</v>
@@ -4493,7 +4535,7 @@
         <v>13</v>
       </c>
       <c r="I107" s="46" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="J107" s="47"/>
     </row>
@@ -4509,10 +4551,10 @@
         <v>8</v>
       </c>
       <c r="D108" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E108" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F108" s="42" t="n">
         <v>1</v>
@@ -4524,10 +4566,10 @@
         <v>13</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J108" s="42" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
     <row r="109" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4542,10 +4584,10 @@
         <v>8</v>
       </c>
       <c r="D109" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E109" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F109" s="42" t="n">
         <v>2</v>
@@ -4557,7 +4599,7 @@
         <v>13</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J109" s="38"/>
       <c r="K109" s="38"/>
@@ -4590,10 +4632,10 @@
         <v>8</v>
       </c>
       <c r="D110" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E110" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F110" s="42" t="n">
         <v>3</v>
@@ -4605,7 +4647,7 @@
         <v>13</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J110" s="38"/>
       <c r="K110" s="38"/>
@@ -4638,10 +4680,10 @@
         <v>8</v>
       </c>
       <c r="D111" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E111" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F111" s="42" t="n">
         <v>4</v>
@@ -4653,7 +4695,7 @@
         <v>13</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J111" s="38"/>
       <c r="K111" s="38"/>
@@ -4686,10 +4728,10 @@
         <v>8</v>
       </c>
       <c r="D112" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E112" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F112" s="42" t="n">
         <v>5</v>
@@ -4701,7 +4743,7 @@
         <v>13</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J112" s="38"/>
       <c r="K112" s="38"/>
@@ -4734,10 +4776,10 @@
         <v>8</v>
       </c>
       <c r="D113" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E113" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F113" s="42" t="n">
         <v>6</v>
@@ -4749,7 +4791,7 @@
         <v>13</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J113" s="38"/>
       <c r="K113" s="38"/>
@@ -4782,10 +4824,10 @@
         <v>8</v>
       </c>
       <c r="D114" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E114" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F114" s="42" t="n">
         <v>7</v>
@@ -4797,7 +4839,7 @@
         <v>13</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J114" s="38"/>
       <c r="K114" s="38"/>
@@ -4830,10 +4872,10 @@
         <v>8</v>
       </c>
       <c r="D115" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E115" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F115" s="42" t="n">
         <v>8</v>
@@ -4845,7 +4887,7 @@
         <v>13</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J115" s="38"/>
       <c r="K115" s="38"/>
@@ -4878,10 +4920,10 @@
         <v>8</v>
       </c>
       <c r="D116" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E116" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F116" s="42" t="n">
         <v>9</v>
@@ -4893,7 +4935,7 @@
         <v>13</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J116" s="38"/>
       <c r="K116" s="38"/>
@@ -4926,10 +4968,10 @@
         <v>8</v>
       </c>
       <c r="D117" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E117" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F117" s="42" t="n">
         <v>10</v>
@@ -4941,7 +4983,7 @@
         <v>13</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J117" s="38"/>
       <c r="K117" s="38"/>
@@ -4974,10 +5016,10 @@
         <v>8</v>
       </c>
       <c r="D118" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E118" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F118" s="42" t="n">
         <v>11</v>
@@ -4989,10 +5031,10 @@
         <v>13</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J118" s="42" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
     <row r="119" s="16" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5007,10 +5049,10 @@
         <v>8</v>
       </c>
       <c r="D119" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E119" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F119" s="42" t="n">
         <v>12</v>
@@ -5022,7 +5064,7 @@
         <v>13</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J119" s="38"/>
       <c r="K119" s="38"/>
@@ -5055,10 +5097,10 @@
         <v>8</v>
       </c>
       <c r="D120" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E120" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F120" s="42" t="n">
         <v>13</v>
@@ -5070,7 +5112,7 @@
         <v>13</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J120" s="38"/>
       <c r="K120" s="38"/>
@@ -5103,10 +5145,10 @@
         <v>8</v>
       </c>
       <c r="D121" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E121" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F121" s="42" t="n">
         <v>14</v>
@@ -5118,7 +5160,7 @@
         <v>13</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J121" s="38"/>
       <c r="K121" s="38"/>
@@ -5151,10 +5193,10 @@
         <v>8</v>
       </c>
       <c r="D122" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E122" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F122" s="42" t="n">
         <v>15</v>
@@ -5166,7 +5208,7 @@
         <v>13</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J122" s="38"/>
       <c r="K122" s="38"/>
@@ -5199,10 +5241,10 @@
         <v>8</v>
       </c>
       <c r="D123" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E123" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F123" s="42" t="n">
         <v>16</v>
@@ -5214,7 +5256,7 @@
         <v>13</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J123" s="38"/>
       <c r="K123" s="38"/>
@@ -5247,10 +5289,10 @@
         <v>8</v>
       </c>
       <c r="D124" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E124" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F124" s="42" t="n">
         <v>17</v>
@@ -5262,7 +5304,7 @@
         <v>13</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J124" s="38"/>
       <c r="K124" s="38"/>
@@ -5295,10 +5337,10 @@
         <v>8</v>
       </c>
       <c r="D125" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E125" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F125" s="42" t="n">
         <v>18</v>
@@ -5310,7 +5352,7 @@
         <v>13</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J125" s="38"/>
       <c r="K125" s="38"/>
@@ -5343,10 +5385,10 @@
         <v>8</v>
       </c>
       <c r="D126" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E126" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F126" s="42" t="n">
         <v>19</v>
@@ -5358,7 +5400,7 @@
         <v>13</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J126" s="38"/>
       <c r="K126" s="38"/>
@@ -5391,10 +5433,10 @@
         <v>8</v>
       </c>
       <c r="D127" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E127" s="48" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="F127" s="42" t="n">
         <v>20</v>
@@ -5406,7 +5448,7 @@
         <v>13</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J127" s="38"/>
       <c r="K127" s="38"/>
@@ -5439,7 +5481,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E128" s="32" t="s">
         <v>5</v>
@@ -5454,7 +5496,7 @@
         <v>13</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J128" s="38"/>
       <c r="K128" s="38"/>
@@ -5487,7 +5529,7 @@
         <v>8</v>
       </c>
       <c r="D129" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E129" s="32" t="s">
         <v>5</v>
@@ -5502,7 +5544,7 @@
         <v>13</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J129" s="38"/>
       <c r="K129" s="38"/>
@@ -5535,7 +5577,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E130" s="32" t="s">
         <v>5</v>
@@ -5550,7 +5592,7 @@
         <v>13</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J130" s="38"/>
       <c r="K130" s="38"/>
@@ -5583,7 +5625,7 @@
         <v>8</v>
       </c>
       <c r="D131" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E131" s="32" t="s">
         <v>5</v>
@@ -5598,7 +5640,7 @@
         <v>13</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J131" s="38"/>
       <c r="K131" s="38"/>
@@ -5631,7 +5673,7 @@
         <v>8</v>
       </c>
       <c r="D132" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E132" s="32" t="s">
         <v>5</v>
@@ -5646,7 +5688,7 @@
         <v>13</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J132" s="38"/>
       <c r="K132" s="38"/>
@@ -5679,7 +5721,7 @@
         <v>8</v>
       </c>
       <c r="D133" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E133" s="32" t="s">
         <v>5</v>
@@ -5694,7 +5736,7 @@
         <v>13</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J133" s="38"/>
       <c r="K133" s="38"/>
@@ -5727,7 +5769,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E134" s="32" t="s">
         <v>5</v>
@@ -5742,7 +5784,7 @@
         <v>13</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J134" s="38"/>
       <c r="K134" s="38"/>
@@ -5775,7 +5817,7 @@
         <v>8</v>
       </c>
       <c r="D135" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E135" s="32" t="s">
         <v>5</v>
@@ -5790,7 +5832,7 @@
         <v>13</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J135" s="38"/>
       <c r="K135" s="38"/>
@@ -5823,7 +5865,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E136" s="32" t="s">
         <v>5</v>
@@ -5838,7 +5880,7 @@
         <v>13</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J136" s="38"/>
       <c r="K136" s="38"/>
@@ -5871,7 +5913,7 @@
         <v>8</v>
       </c>
       <c r="D137" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E137" s="32" t="s">
         <v>5</v>
@@ -5886,7 +5928,7 @@
         <v>13</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J137" s="38"/>
       <c r="K137" s="38"/>
@@ -5919,7 +5961,7 @@
         <v>8</v>
       </c>
       <c r="D138" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E138" s="32" t="s">
         <v>5</v>
@@ -5934,7 +5976,7 @@
         <v>13</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J138" s="38"/>
       <c r="K138" s="38"/>
@@ -5967,7 +6009,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E139" s="32" t="s">
         <v>5</v>
@@ -5982,7 +6024,7 @@
         <v>13</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J139" s="38"/>
       <c r="K139" s="38"/>
@@ -6015,7 +6057,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E140" s="32" t="s">
         <v>5</v>
@@ -6030,7 +6072,7 @@
         <v>13</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J140" s="38"/>
       <c r="K140" s="38"/>
@@ -6063,7 +6105,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E141" s="32" t="s">
         <v>5</v>
@@ -6078,7 +6120,7 @@
         <v>13</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J141" s="38"/>
       <c r="K141" s="38"/>
@@ -6111,7 +6153,7 @@
         <v>8</v>
       </c>
       <c r="D142" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E142" s="32" t="s">
         <v>5</v>
@@ -6126,7 +6168,7 @@
         <v>13</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J142" s="38"/>
       <c r="K142" s="38"/>
@@ -6159,7 +6201,7 @@
         <v>8</v>
       </c>
       <c r="D143" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E143" s="32" t="s">
         <v>5</v>
@@ -6174,7 +6216,7 @@
         <v>13</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J143" s="38"/>
       <c r="K143" s="38"/>
@@ -6207,7 +6249,7 @@
         <v>8</v>
       </c>
       <c r="D144" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E144" s="32" t="s">
         <v>5</v>
@@ -6222,7 +6264,7 @@
         <v>13</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J144" s="38"/>
       <c r="K144" s="38"/>
@@ -6255,7 +6297,7 @@
         <v>8</v>
       </c>
       <c r="D145" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E145" s="32" t="s">
         <v>5</v>
@@ -6270,7 +6312,7 @@
         <v>13</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J145" s="38"/>
       <c r="K145" s="38"/>
@@ -6303,7 +6345,7 @@
         <v>8</v>
       </c>
       <c r="D146" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E146" s="32" t="s">
         <v>5</v>
@@ -6318,7 +6360,7 @@
         <v>13</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J146" s="38"/>
       <c r="K146" s="38"/>
@@ -6351,7 +6393,7 @@
         <v>8</v>
       </c>
       <c r="D147" s="42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E147" s="32" t="s">
         <v>5</v>
@@ -6366,7 +6408,7 @@
         <v>13</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="J147" s="38"/>
       <c r="K147" s="38"/>
@@ -6399,10 +6441,10 @@
         <v>8</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F148" s="30" t="s">
         <v>23</v>
@@ -6414,7 +6456,7 @@
         <v>13</v>
       </c>
       <c r="I148" s="16" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6429,10 +6471,10 @@
         <v>8</v>
       </c>
       <c r="D149" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E149" s="49" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F149" s="37" t="s">
         <v>26</v>
@@ -6444,7 +6486,7 @@
         <v>13</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6459,10 +6501,10 @@
         <v>8</v>
       </c>
       <c r="D150" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E150" s="49" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F150" s="37" t="s">
         <v>27</v>
@@ -6474,7 +6516,7 @@
         <v>13</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6489,10 +6531,10 @@
         <v>8</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E151" s="49" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F151" s="37" t="s">
         <v>28</v>
@@ -6504,7 +6546,7 @@
         <v>13</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6519,10 +6561,10 @@
         <v>8</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E152" s="49" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F152" s="37" t="s">
         <v>29</v>
@@ -6534,7 +6576,7 @@
         <v>13</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6549,13 +6591,13 @@
         <v>8</v>
       </c>
       <c r="D153" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E153" s="49" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="F153" s="37" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="G153" s="37" t="s">
         <v>8</v>
@@ -6564,7 +6606,7 @@
         <v>13</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6579,10 +6621,10 @@
         <v>8</v>
       </c>
       <c r="D154" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E154" s="50" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="F154" s="37" t="s">
         <v>23</v>
@@ -6594,7 +6636,7 @@
         <v>13</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6609,10 +6651,10 @@
         <v>8</v>
       </c>
       <c r="D155" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E155" s="50" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="F155" s="37" t="s">
         <v>26</v>
@@ -6624,7 +6666,7 @@
         <v>13</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6639,10 +6681,10 @@
         <v>8</v>
       </c>
       <c r="D156" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E156" s="50" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="F156" s="37" t="s">
         <v>27</v>
@@ -6654,7 +6696,7 @@
         <v>13</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6669,10 +6711,10 @@
         <v>8</v>
       </c>
       <c r="D157" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E157" s="50" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="F157" s="37" t="s">
         <v>28</v>
@@ -6684,7 +6726,7 @@
         <v>13</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6699,10 +6741,10 @@
         <v>8</v>
       </c>
       <c r="D158" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E158" s="50" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="F158" s="37" t="s">
         <v>29</v>
@@ -6714,7 +6756,7 @@
         <v>13</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6729,13 +6771,13 @@
         <v>8</v>
       </c>
       <c r="D159" s="22" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E159" s="50" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="F159" s="37" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="G159" s="37" t="s">
         <v>8</v>
@@ -6744,7 +6786,7 @@
         <v>13</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6759,7 +6801,7 @@
         <v>8</v>
       </c>
       <c r="D160" s="45" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E160" s="50" t="n">
         <v>1</v>
@@ -6774,7 +6816,7 @@
         <v>13</v>
       </c>
       <c r="I160" s="52" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6789,7 +6831,7 @@
         <v>8</v>
       </c>
       <c r="D161" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E161" s="53" t="n">
         <v>2</v>
@@ -6804,7 +6846,7 @@
         <v>13</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6819,7 +6861,7 @@
         <v>8</v>
       </c>
       <c r="D162" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E162" s="53" t="n">
         <v>3</v>
@@ -6834,7 +6876,7 @@
         <v>13</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6849,7 +6891,7 @@
         <v>8</v>
       </c>
       <c r="D163" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E163" s="53" t="n">
         <v>4</v>
@@ -6864,7 +6906,7 @@
         <v>13</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6879,7 +6921,7 @@
         <v>8</v>
       </c>
       <c r="D164" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E164" s="53" t="n">
         <v>5</v>
@@ -6894,7 +6936,7 @@
         <v>13</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6909,7 +6951,7 @@
         <v>8</v>
       </c>
       <c r="D165" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E165" s="53" t="n">
         <v>6</v>
@@ -6924,7 +6966,7 @@
         <v>13</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6939,7 +6981,7 @@
         <v>8</v>
       </c>
       <c r="D166" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E166" s="53" t="n">
         <v>7</v>
@@ -6954,7 +6996,7 @@
         <v>13</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6969,7 +7011,7 @@
         <v>8</v>
       </c>
       <c r="D167" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E167" s="53" t="n">
         <v>8</v>
@@ -6984,7 +7026,7 @@
         <v>13</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6999,7 +7041,7 @@
         <v>8</v>
       </c>
       <c r="D168" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E168" s="53" t="n">
         <v>9</v>
@@ -7014,7 +7056,7 @@
         <v>13</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7029,7 +7071,7 @@
         <v>8</v>
       </c>
       <c r="D169" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E169" s="53" t="n">
         <v>10</v>
@@ -7044,7 +7086,7 @@
         <v>13</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7059,7 +7101,7 @@
         <v>8</v>
       </c>
       <c r="D170" s="45" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E170" s="50" t="n">
         <v>11</v>
@@ -7074,7 +7116,7 @@
         <v>13</v>
       </c>
       <c r="I170" s="52" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7089,7 +7131,7 @@
         <v>8</v>
       </c>
       <c r="D171" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E171" s="53" t="n">
         <v>12</v>
@@ -7104,7 +7146,7 @@
         <v>13</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7119,7 +7161,7 @@
         <v>8</v>
       </c>
       <c r="D172" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E172" s="53" t="n">
         <v>13</v>
@@ -7134,7 +7176,7 @@
         <v>13</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7149,7 +7191,7 @@
         <v>8</v>
       </c>
       <c r="D173" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E173" s="53" t="n">
         <v>14</v>
@@ -7164,7 +7206,7 @@
         <v>13</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7179,7 +7221,7 @@
         <v>8</v>
       </c>
       <c r="D174" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E174" s="53" t="n">
         <v>15</v>
@@ -7194,7 +7236,7 @@
         <v>13</v>
       </c>
       <c r="I174" s="52" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7209,7 +7251,7 @@
         <v>8</v>
       </c>
       <c r="D175" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E175" s="50" t="n">
         <v>16</v>
@@ -7224,7 +7266,7 @@
         <v>13</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7239,7 +7281,7 @@
         <v>8</v>
       </c>
       <c r="D176" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E176" s="53" t="n">
         <v>17</v>
@@ -7254,7 +7296,7 @@
         <v>13</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7269,7 +7311,7 @@
         <v>8</v>
       </c>
       <c r="D177" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E177" s="53" t="n">
         <v>18</v>
@@ -7284,7 +7326,7 @@
         <v>13</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7299,7 +7341,7 @@
         <v>8</v>
       </c>
       <c r="D178" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E178" s="53" t="n">
         <v>19</v>
@@ -7314,7 +7356,7 @@
         <v>13</v>
       </c>
       <c r="I178" s="52" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7329,7 +7371,7 @@
         <v>8</v>
       </c>
       <c r="D179" s="42" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E179" s="53" t="n">
         <v>20</v>
@@ -7344,7 +7386,7 @@
         <v>13</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
     </row>
     <row r="180" s="52" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7359,10 +7401,10 @@
         <v>8</v>
       </c>
       <c r="D180" s="45" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E180" s="50" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F180" s="51" t="n">
         <v>1</v>
@@ -7374,7 +7416,7 @@
         <v>13</v>
       </c>
       <c r="I180" s="52" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7389,10 +7431,10 @@
         <v>8</v>
       </c>
       <c r="D181" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E181" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F181" s="37" t="n">
         <v>2</v>
@@ -7404,7 +7446,7 @@
         <v>13</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7419,10 +7461,10 @@
         <v>8</v>
       </c>
       <c r="D182" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E182" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F182" s="37" t="n">
         <v>3</v>
@@ -7434,7 +7476,7 @@
         <v>13</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7449,10 +7491,10 @@
         <v>8</v>
       </c>
       <c r="D183" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E183" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F183" s="37" t="n">
         <v>4</v>
@@ -7464,7 +7506,7 @@
         <v>13</v>
       </c>
       <c r="I183" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7479,10 +7521,10 @@
         <v>8</v>
       </c>
       <c r="D184" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E184" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F184" s="37" t="n">
         <v>5</v>
@@ -7494,7 +7536,7 @@
         <v>13</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7509,10 +7551,10 @@
         <v>8</v>
       </c>
       <c r="D185" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E185" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F185" s="37" t="n">
         <v>6</v>
@@ -7524,7 +7566,7 @@
         <v>13</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7539,10 +7581,10 @@
         <v>8</v>
       </c>
       <c r="D186" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E186" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F186" s="37" t="n">
         <v>7</v>
@@ -7554,7 +7596,7 @@
         <v>13</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7569,10 +7611,10 @@
         <v>8</v>
       </c>
       <c r="D187" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E187" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F187" s="37" t="n">
         <v>8</v>
@@ -7584,7 +7626,7 @@
         <v>13</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7599,10 +7641,10 @@
         <v>8</v>
       </c>
       <c r="D188" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E188" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F188" s="37" t="n">
         <v>9</v>
@@ -7614,7 +7656,7 @@
         <v>13</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7629,10 +7671,10 @@
         <v>8</v>
       </c>
       <c r="D189" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E189" s="54" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="F189" s="37" t="n">
         <v>10</v>
@@ -7644,7 +7686,7 @@
         <v>13</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="190" s="52" customFormat="true" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7659,10 +7701,10 @@
         <v>8</v>
       </c>
       <c r="D190" s="45" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E190" s="50" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F190" s="51" t="n">
         <v>1</v>
@@ -7674,7 +7716,7 @@
         <v>13</v>
       </c>
       <c r="I190" s="52" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7689,10 +7731,10 @@
         <v>8</v>
       </c>
       <c r="D191" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E191" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F191" s="37" t="n">
         <v>2</v>
@@ -7704,7 +7746,7 @@
         <v>13</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7719,10 +7761,10 @@
         <v>8</v>
       </c>
       <c r="D192" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E192" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F192" s="37" t="n">
         <v>3</v>
@@ -7734,7 +7776,7 @@
         <v>13</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7749,10 +7791,10 @@
         <v>8</v>
       </c>
       <c r="D193" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E193" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F193" s="37" t="n">
         <v>4</v>
@@ -7764,7 +7806,7 @@
         <v>13</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7779,10 +7821,10 @@
         <v>8</v>
       </c>
       <c r="D194" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E194" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F194" s="37" t="n">
         <v>5</v>
@@ -7794,7 +7836,7 @@
         <v>13</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7809,10 +7851,10 @@
         <v>8</v>
       </c>
       <c r="D195" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E195" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F195" s="37" t="n">
         <v>6</v>
@@ -7824,7 +7866,7 @@
         <v>13</v>
       </c>
       <c r="I195" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7839,10 +7881,10 @@
         <v>8</v>
       </c>
       <c r="D196" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E196" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F196" s="37" t="n">
         <v>7</v>
@@ -7854,7 +7896,7 @@
         <v>13</v>
       </c>
       <c r="I196" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7869,10 +7911,10 @@
         <v>8</v>
       </c>
       <c r="D197" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E197" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F197" s="37" t="n">
         <v>8</v>
@@ -7884,7 +7926,7 @@
         <v>13</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7899,10 +7941,10 @@
         <v>8</v>
       </c>
       <c r="D198" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E198" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F198" s="37" t="n">
         <v>9</v>
@@ -7914,7 +7956,7 @@
         <v>13</v>
       </c>
       <c r="I198" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7929,10 +7971,10 @@
         <v>8</v>
       </c>
       <c r="D199" s="22" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E199" s="55" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="F199" s="37" t="n">
         <v>10</v>
@@ -7944,7 +7986,7 @@
         <v>13</v>
       </c>
       <c r="I199" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="200" s="52" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7959,13 +8001,13 @@
         <v>8</v>
       </c>
       <c r="D200" s="45" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E200" s="50" t="n">
         <v>1</v>
       </c>
       <c r="F200" s="50" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="G200" s="50" t="s">
         <v>8</v>
@@ -7974,7 +8016,7 @@
         <v>13</v>
       </c>
       <c r="I200" s="52" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7989,13 +8031,13 @@
         <v>8</v>
       </c>
       <c r="D201" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E201" s="53" t="n">
         <v>1</v>
       </c>
       <c r="F201" s="53" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="G201" s="53" t="s">
         <v>8</v>
@@ -8004,7 +8046,7 @@
         <v>13</v>
       </c>
       <c r="I201" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8019,13 +8061,13 @@
         <v>8</v>
       </c>
       <c r="D202" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E202" s="53" t="n">
         <v>1</v>
       </c>
       <c r="F202" s="53" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="G202" s="53" t="s">
         <v>8</v>
@@ -8034,7 +8076,7 @@
         <v>13</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8049,13 +8091,13 @@
         <v>8</v>
       </c>
       <c r="D203" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E203" s="53" t="n">
         <v>1</v>
       </c>
       <c r="F203" s="53" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="G203" s="53" t="s">
         <v>8</v>
@@ -8064,7 +8106,7 @@
         <v>13</v>
       </c>
       <c r="I203" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8079,13 +8121,13 @@
         <v>8</v>
       </c>
       <c r="D204" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E204" s="53" t="n">
         <v>2</v>
       </c>
       <c r="F204" s="53" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="G204" s="53" t="s">
         <v>8</v>
@@ -8094,7 +8136,7 @@
         <v>13</v>
       </c>
       <c r="I204" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8109,13 +8151,13 @@
         <v>8</v>
       </c>
       <c r="D205" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E205" s="53" t="n">
         <v>2</v>
       </c>
       <c r="F205" s="53" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="G205" s="53" t="s">
         <v>8</v>
@@ -8124,7 +8166,7 @@
         <v>13</v>
       </c>
       <c r="I205" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8139,13 +8181,13 @@
         <v>8</v>
       </c>
       <c r="D206" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E206" s="53" t="n">
         <v>2</v>
       </c>
       <c r="F206" s="53" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="G206" s="53" t="s">
         <v>8</v>
@@ -8154,7 +8196,7 @@
         <v>13</v>
       </c>
       <c r="I206" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8169,13 +8211,13 @@
         <v>8</v>
       </c>
       <c r="D207" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E207" s="53" t="n">
         <v>2</v>
       </c>
       <c r="F207" s="53" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="G207" s="53" t="s">
         <v>8</v>
@@ -8184,7 +8226,7 @@
         <v>13</v>
       </c>
       <c r="I207" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8199,13 +8241,13 @@
         <v>8</v>
       </c>
       <c r="D208" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E208" s="53" t="n">
         <v>3</v>
       </c>
       <c r="F208" s="53" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="G208" s="53" t="s">
         <v>8</v>
@@ -8214,7 +8256,7 @@
         <v>13</v>
       </c>
       <c r="I208" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8229,13 +8271,13 @@
         <v>8</v>
       </c>
       <c r="D209" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E209" s="53" t="n">
         <v>3</v>
       </c>
       <c r="F209" s="53" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="G209" s="53" t="s">
         <v>8</v>
@@ -8244,7 +8286,7 @@
         <v>13</v>
       </c>
       <c r="I209" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8259,13 +8301,13 @@
         <v>8</v>
       </c>
       <c r="D210" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E210" s="53" t="n">
         <v>3</v>
       </c>
       <c r="F210" s="53" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="G210" s="53" t="s">
         <v>8</v>
@@ -8274,7 +8316,7 @@
         <v>13</v>
       </c>
       <c r="I210" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8289,13 +8331,13 @@
         <v>8</v>
       </c>
       <c r="D211" s="42" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E211" s="53" t="n">
         <v>3</v>
       </c>
       <c r="F211" s="53" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="G211" s="53" t="s">
         <v>8</v>
@@ -8304,7 +8346,7 @@
         <v>13</v>
       </c>
       <c r="I211" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="212" s="52" customFormat="true" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8319,13 +8361,13 @@
         <v>8</v>
       </c>
       <c r="D212" s="45" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="E212" s="50" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="F212" s="50" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="G212" s="51" t="s">
         <v>8</v>
@@ -8334,7 +8376,7 @@
         <v>13</v>
       </c>
       <c r="I212" s="52" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
     </row>
     <row r="213" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Ökobilanzielle Bewertung textarea added
</commit_message>
<xml_diff>
--- a/R2Q_Datensatz_leer.xlsx
+++ b/R2Q_Datensatz_leer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flemming\Google Drive\R\R2Q_App\R2Q_App_VCurrent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3DB272-C0A1-4384-9D1E-8CF65B7AC1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776D8FB5-8FDB-4C80-ABA6-7304D81A7614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Musterdatensatz" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="243">
   <si>
     <t>ID</t>
   </si>
@@ -760,6 +760,9 @@
   </si>
   <si>
     <t>bewertung</t>
+  </si>
+  <si>
+    <t>bewertungText</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1066,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1233,15 +1236,6 @@
     <xf numFmtId="0" fontId="7" fillId="17" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1250,6 +1244,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1635,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ232"/>
+  <dimension ref="A1:AMJ233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J171" sqref="J171"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J160" sqref="J160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15"/>
@@ -6321,7 +6330,7 @@
     </row>
     <row r="139" spans="1:27" s="16" customFormat="1" ht="17.25">
       <c r="A139" s="9">
-        <f t="shared" ref="A139:A190" si="5">ROW(A139)-1</f>
+        <f t="shared" ref="A139:A191" si="5">ROW(A139)-1</f>
         <v>138</v>
       </c>
       <c r="B139" s="9" t="s">
@@ -7081,7 +7090,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="159" spans="1:27" ht="30">
+    <row r="159" spans="1:27" ht="31.5" thickTop="1" thickBot="1">
       <c r="A159" s="9">
         <f t="shared" si="5"/>
         <v>158</v>
@@ -7111,7 +7120,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="160" spans="1:27" ht="17.25">
+    <row r="160" spans="1:27" ht="18.75" thickTop="1" thickBot="1">
       <c r="A160" s="9">
         <f t="shared" si="5"/>
         <v>159</v>
@@ -7125,24 +7134,23 @@
       <c r="D160" s="56" t="s">
         <v>238</v>
       </c>
-      <c r="E160" s="57" t="s">
-        <v>239</v>
-      </c>
-      <c r="F160" s="58">
-        <v>1</v>
-      </c>
-      <c r="G160" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="H160" s="58" t="s">
-        <v>13</v>
-      </c>
-      <c r="I160" s="59" t="s">
-        <v>241</v>
-      </c>
-      <c r="J160" s="59"/>
-    </row>
-    <row r="161" spans="1:9" ht="17.25">
+      <c r="E160" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="F160" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="G160" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="H160" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="I160" s="64" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="18.75" thickTop="1" thickBot="1">
       <c r="A161" s="9">
         <f t="shared" si="5"/>
         <v>160</v>
@@ -7153,26 +7161,27 @@
       <c r="C161" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D161" s="22" t="s">
+      <c r="D161" s="60" t="s">
         <v>238</v>
       </c>
-      <c r="E161" s="61" t="s">
+      <c r="E161" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="F161" s="37">
-        <v>2</v>
-      </c>
-      <c r="G161" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H161" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I161" s="1" t="s">
+      <c r="F161" s="57">
+        <v>1</v>
+      </c>
+      <c r="G161" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="H161" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="I161" s="61" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" ht="17.25">
+      <c r="J161" s="61"/>
+    </row>
+    <row r="162" spans="1:10" ht="17.25">
       <c r="A162" s="9">
         <f t="shared" si="5"/>
         <v>161</v>
@@ -7186,23 +7195,23 @@
       <c r="D162" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E162" s="61" t="s">
+      <c r="E162" s="58" t="s">
         <v>239</v>
       </c>
       <c r="F162" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G162" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H162" s="37" t="s">
-        <v>13</v>
+      <c r="H162" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="17.25">
+    <row r="163" spans="1:10" ht="17.25">
       <c r="A163" s="9">
         <f t="shared" si="5"/>
         <v>162</v>
@@ -7216,23 +7225,23 @@
       <c r="D163" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E163" s="61" t="s">
+      <c r="E163" s="58" t="s">
         <v>239</v>
       </c>
       <c r="F163" s="37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G163" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H163" s="37" t="s">
-        <v>13</v>
+      <c r="H163" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I163" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="17.25">
+    <row r="164" spans="1:10" ht="17.25">
       <c r="A164" s="9">
         <f t="shared" si="5"/>
         <v>163</v>
@@ -7246,23 +7255,23 @@
       <c r="D164" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E164" s="61" t="s">
+      <c r="E164" s="58" t="s">
         <v>239</v>
       </c>
       <c r="F164" s="37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G164" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H164" s="37" t="s">
-        <v>13</v>
+      <c r="H164" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="17.25">
+    <row r="165" spans="1:10" ht="17.25">
       <c r="A165" s="9">
         <f t="shared" si="5"/>
         <v>164</v>
@@ -7276,23 +7285,23 @@
       <c r="D165" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E165" s="61" t="s">
+      <c r="E165" s="58" t="s">
         <v>239</v>
       </c>
       <c r="F165" s="37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G165" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H165" s="37" t="s">
-        <v>13</v>
+      <c r="H165" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="17.25">
+    <row r="166" spans="1:10" ht="17.25">
       <c r="A166" s="9">
         <f t="shared" si="5"/>
         <v>165</v>
@@ -7306,23 +7315,23 @@
       <c r="D166" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E166" s="61" t="s">
+      <c r="E166" s="58" t="s">
         <v>239</v>
       </c>
       <c r="F166" s="37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G166" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H166" s="37" t="s">
-        <v>13</v>
+      <c r="H166" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="17.25">
+    <row r="167" spans="1:10" ht="17.25">
       <c r="A167" s="9">
         <f t="shared" si="5"/>
         <v>166</v>
@@ -7336,23 +7345,23 @@
       <c r="D167" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E167" s="61" t="s">
+      <c r="E167" s="58" t="s">
         <v>239</v>
       </c>
       <c r="F167" s="37">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G167" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H167" s="37" t="s">
-        <v>13</v>
+      <c r="H167" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I167" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="17.25">
+    <row r="168" spans="1:10" ht="17.25">
       <c r="A168" s="9">
         <f t="shared" si="5"/>
         <v>167</v>
@@ -7366,23 +7375,23 @@
       <c r="D168" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E168" s="61" t="s">
+      <c r="E168" s="58" t="s">
         <v>239</v>
       </c>
       <c r="F168" s="37">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G168" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H168" s="37" t="s">
-        <v>13</v>
+      <c r="H168" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I168" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="17.25">
+    <row r="169" spans="1:10" ht="17.25">
       <c r="A169" s="9">
         <f t="shared" si="5"/>
         <v>168</v>
@@ -7396,23 +7405,23 @@
       <c r="D169" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E169" s="61" t="s">
+      <c r="E169" s="58" t="s">
         <v>239</v>
       </c>
       <c r="F169" s="37">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G169" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H169" s="37" t="s">
-        <v>13</v>
+      <c r="H169" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I169" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="17.25">
+    <row r="170" spans="1:10" ht="17.25">
       <c r="A170" s="9">
         <f t="shared" si="5"/>
         <v>169</v>
@@ -7426,23 +7435,23 @@
       <c r="D170" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E170" s="62" t="s">
-        <v>240</v>
-      </c>
-      <c r="F170" s="60">
-        <v>1</v>
+      <c r="E170" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="F170" s="37">
+        <v>10</v>
       </c>
       <c r="G170" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H170" s="37" t="s">
-        <v>13</v>
+      <c r="H170" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I170" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="17.25">
+    <row r="171" spans="1:10" ht="17.25">
       <c r="A171" s="9">
         <f t="shared" si="5"/>
         <v>170</v>
@@ -7456,23 +7465,23 @@
       <c r="D171" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E171" s="62" t="s">
+      <c r="E171" s="59" t="s">
         <v>240</v>
       </c>
-      <c r="F171" s="37">
-        <v>2</v>
+      <c r="F171" s="57">
+        <v>1</v>
       </c>
       <c r="G171" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H171" s="37" t="s">
-        <v>13</v>
+      <c r="H171" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I171" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="17.25">
+    <row r="172" spans="1:10" ht="17.25">
       <c r="A172" s="9">
         <f t="shared" si="5"/>
         <v>171</v>
@@ -7486,23 +7495,23 @@
       <c r="D172" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E172" s="62" t="s">
+      <c r="E172" s="59" t="s">
         <v>240</v>
       </c>
       <c r="F172" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G172" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H172" s="37" t="s">
-        <v>13</v>
+      <c r="H172" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I172" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="17.25">
+    <row r="173" spans="1:10" ht="17.25">
       <c r="A173" s="9">
         <f t="shared" si="5"/>
         <v>172</v>
@@ -7516,23 +7525,23 @@
       <c r="D173" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E173" s="62" t="s">
+      <c r="E173" s="59" t="s">
         <v>240</v>
       </c>
       <c r="F173" s="37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G173" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H173" s="37" t="s">
-        <v>13</v>
+      <c r="H173" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I173" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="17.25">
+    <row r="174" spans="1:10" ht="17.25">
       <c r="A174" s="9">
         <f t="shared" si="5"/>
         <v>173</v>
@@ -7546,23 +7555,23 @@
       <c r="D174" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E174" s="62" t="s">
+      <c r="E174" s="59" t="s">
         <v>240</v>
       </c>
       <c r="F174" s="37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G174" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H174" s="37" t="s">
-        <v>13</v>
+      <c r="H174" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I174" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="17.25">
+    <row r="175" spans="1:10" ht="17.25">
       <c r="A175" s="9">
         <f t="shared" si="5"/>
         <v>174</v>
@@ -7576,23 +7585,23 @@
       <c r="D175" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E175" s="62" t="s">
+      <c r="E175" s="59" t="s">
         <v>240</v>
       </c>
       <c r="F175" s="37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G175" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H175" s="37" t="s">
-        <v>13</v>
+      <c r="H175" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I175" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="17.25">
+    <row r="176" spans="1:10" ht="17.25">
       <c r="A176" s="9">
         <f t="shared" si="5"/>
         <v>175</v>
@@ -7606,17 +7615,17 @@
       <c r="D176" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E176" s="62" t="s">
+      <c r="E176" s="59" t="s">
         <v>240</v>
       </c>
       <c r="F176" s="37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G176" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H176" s="37" t="s">
-        <v>13</v>
+      <c r="H176" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I176" s="1" t="s">
         <v>241</v>
@@ -7636,17 +7645,17 @@
       <c r="D177" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E177" s="62" t="s">
+      <c r="E177" s="59" t="s">
         <v>240</v>
       </c>
       <c r="F177" s="37">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G177" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H177" s="37" t="s">
-        <v>13</v>
+      <c r="H177" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I177" s="1" t="s">
         <v>241</v>
@@ -7666,17 +7675,17 @@
       <c r="D178" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E178" s="62" t="s">
+      <c r="E178" s="59" t="s">
         <v>240</v>
       </c>
       <c r="F178" s="37">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G178" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H178" s="37" t="s">
-        <v>13</v>
+      <c r="H178" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I178" s="1" t="s">
         <v>241</v>
@@ -7696,17 +7705,17 @@
       <c r="D179" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E179" s="62" t="s">
+      <c r="E179" s="59" t="s">
         <v>240</v>
       </c>
       <c r="F179" s="37">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G179" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H179" s="37" t="s">
-        <v>13</v>
+      <c r="H179" s="57" t="s">
+        <v>89</v>
       </c>
       <c r="I179" s="1" t="s">
         <v>241</v>
@@ -7723,23 +7732,23 @@
       <c r="C180" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D180" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="E180" s="50">
-        <v>1</v>
-      </c>
-      <c r="F180" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="G180" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="H180" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="I180" s="52" t="s">
-        <v>205</v>
+      <c r="D180" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="E180" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="F180" s="37">
+        <v>10</v>
+      </c>
+      <c r="G180" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H180" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="17.25">
@@ -7753,23 +7762,23 @@
       <c r="C181" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D181" s="42" t="s">
+      <c r="D181" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="E181" s="53">
-        <v>2</v>
-      </c>
-      <c r="F181" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="G181" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H181" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I181" s="1" t="s">
-        <v>206</v>
+      <c r="E181" s="50">
+        <v>1</v>
+      </c>
+      <c r="F181" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G181" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="H181" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I181" s="52" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="17.25">
@@ -7787,7 +7796,7 @@
         <v>204</v>
       </c>
       <c r="E182" s="53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F182" s="53" t="s">
         <v>8</v>
@@ -7799,7 +7808,7 @@
         <v>13</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="17.25">
@@ -7817,7 +7826,7 @@
         <v>204</v>
       </c>
       <c r="E183" s="53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F183" s="53" t="s">
         <v>8</v>
@@ -7829,7 +7838,7 @@
         <v>13</v>
       </c>
       <c r="I183" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="17.25">
@@ -7847,7 +7856,7 @@
         <v>204</v>
       </c>
       <c r="E184" s="53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F184" s="53" t="s">
         <v>8</v>
@@ -7859,7 +7868,7 @@
         <v>13</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="17.25">
@@ -7877,7 +7886,7 @@
         <v>204</v>
       </c>
       <c r="E185" s="53">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F185" s="53" t="s">
         <v>8</v>
@@ -7889,7 +7898,7 @@
         <v>13</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="17.25">
@@ -7907,7 +7916,7 @@
         <v>204</v>
       </c>
       <c r="E186" s="53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F186" s="53" t="s">
         <v>8</v>
@@ -7919,7 +7928,7 @@
         <v>13</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="17.25">
@@ -7937,7 +7946,7 @@
         <v>204</v>
       </c>
       <c r="E187" s="53">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F187" s="53" t="s">
         <v>8</v>
@@ -7949,7 +7958,7 @@
         <v>13</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="17.25">
@@ -7967,7 +7976,7 @@
         <v>204</v>
       </c>
       <c r="E188" s="53">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F188" s="53" t="s">
         <v>8</v>
@@ -7979,7 +7988,7 @@
         <v>13</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="17.25">
@@ -7997,7 +8006,7 @@
         <v>204</v>
       </c>
       <c r="E189" s="53">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F189" s="53" t="s">
         <v>8</v>
@@ -8009,7 +8018,7 @@
         <v>13</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="17.25">
@@ -8023,28 +8032,28 @@
       <c r="C190" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D190" s="45" t="s">
+      <c r="D190" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="E190" s="50">
-        <v>11</v>
-      </c>
-      <c r="F190" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="G190" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="H190" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="I190" s="52" t="s">
-        <v>215</v>
+      <c r="E190" s="53">
+        <v>10</v>
+      </c>
+      <c r="F190" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G190" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H190" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="17.25">
       <c r="A191" s="9">
-        <f t="shared" ref="A191:A222" si="6">ROW(A191)-1</f>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="B191" s="9" t="s">
@@ -8053,28 +8062,28 @@
       <c r="C191" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D191" s="42" t="s">
+      <c r="D191" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="E191" s="53">
-        <v>12</v>
-      </c>
-      <c r="F191" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="G191" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H191" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I191" s="1" t="s">
-        <v>216</v>
+      <c r="E191" s="50">
+        <v>11</v>
+      </c>
+      <c r="F191" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G191" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="H191" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I191" s="52" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="192" spans="1:9" ht="17.25">
       <c r="A192" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="A192:A223" si="6">ROW(A192)-1</f>
         <v>191</v>
       </c>
       <c r="B192" s="9" t="s">
@@ -8087,7 +8096,7 @@
         <v>204</v>
       </c>
       <c r="E192" s="53">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F192" s="53" t="s">
         <v>8</v>
@@ -8099,7 +8108,7 @@
         <v>13</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="193" spans="1:9" ht="17.25">
@@ -8117,7 +8126,7 @@
         <v>204</v>
       </c>
       <c r="E193" s="53">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F193" s="53" t="s">
         <v>8</v>
@@ -8129,7 +8138,7 @@
         <v>13</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="194" spans="1:9" ht="17.25">
@@ -8147,7 +8156,7 @@
         <v>204</v>
       </c>
       <c r="E194" s="53">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F194" s="53" t="s">
         <v>8</v>
@@ -8158,8 +8167,8 @@
       <c r="H194" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I194" s="52" t="s">
-        <v>219</v>
+      <c r="I194" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="195" spans="1:9" ht="17.25">
@@ -8176,8 +8185,8 @@
       <c r="D195" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="E195" s="50">
-        <v>16</v>
+      <c r="E195" s="53">
+        <v>15</v>
       </c>
       <c r="F195" s="53" t="s">
         <v>8</v>
@@ -8188,8 +8197,8 @@
       <c r="H195" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I195" s="1" t="s">
-        <v>220</v>
+      <c r="I195" s="52" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="196" spans="1:9" ht="17.25">
@@ -8206,8 +8215,8 @@
       <c r="D196" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="E196" s="53">
-        <v>17</v>
+      <c r="E196" s="50">
+        <v>16</v>
       </c>
       <c r="F196" s="53" t="s">
         <v>8</v>
@@ -8219,7 +8228,7 @@
         <v>13</v>
       </c>
       <c r="I196" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="17.25">
@@ -8237,7 +8246,7 @@
         <v>204</v>
       </c>
       <c r="E197" s="53">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F197" s="53" t="s">
         <v>8</v>
@@ -8249,7 +8258,7 @@
         <v>13</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="17.25">
@@ -8267,7 +8276,7 @@
         <v>204</v>
       </c>
       <c r="E198" s="53">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F198" s="53" t="s">
         <v>8</v>
@@ -8278,8 +8287,8 @@
       <c r="H198" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I198" s="52" t="s">
-        <v>223</v>
+      <c r="I198" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="199" spans="1:9" ht="17.25">
@@ -8297,7 +8306,7 @@
         <v>204</v>
       </c>
       <c r="E199" s="53">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F199" s="53" t="s">
         <v>8</v>
@@ -8308,11 +8317,11 @@
       <c r="H199" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I199" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" s="52" customFormat="1" ht="17.25">
+      <c r="I199" s="52" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="17.25">
       <c r="A200" s="9">
         <f t="shared" si="6"/>
         <v>199</v>
@@ -8323,26 +8332,26 @@
       <c r="C200" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D200" s="45" t="s">
-        <v>225</v>
-      </c>
-      <c r="E200" s="50" t="s">
-        <v>226</v>
-      </c>
-      <c r="F200" s="51">
-        <v>1</v>
-      </c>
-      <c r="G200" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="H200" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="I200" s="52" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" ht="17.25">
+      <c r="D200" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="E200" s="53">
+        <v>20</v>
+      </c>
+      <c r="F200" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G200" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H200" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I200" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" s="52" customFormat="1" ht="17.25">
       <c r="A201" s="9">
         <f t="shared" si="6"/>
         <v>200</v>
@@ -8353,22 +8362,22 @@
       <c r="C201" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D201" s="22" t="s">
+      <c r="D201" s="45" t="s">
         <v>225</v>
       </c>
-      <c r="E201" s="54" t="s">
+      <c r="E201" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="F201" s="37">
-        <v>2</v>
-      </c>
-      <c r="G201" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H201" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I201" s="1" t="s">
+      <c r="F201" s="51">
+        <v>1</v>
+      </c>
+      <c r="G201" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="H201" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I201" s="52" t="s">
         <v>227</v>
       </c>
     </row>
@@ -8390,7 +8399,7 @@
         <v>226</v>
       </c>
       <c r="F202" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G202" s="37" t="s">
         <v>8</v>
@@ -8420,7 +8429,7 @@
         <v>226</v>
       </c>
       <c r="F203" s="37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G203" s="37" t="s">
         <v>8</v>
@@ -8450,7 +8459,7 @@
         <v>226</v>
       </c>
       <c r="F204" s="37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G204" s="37" t="s">
         <v>8</v>
@@ -8480,7 +8489,7 @@
         <v>226</v>
       </c>
       <c r="F205" s="37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G205" s="37" t="s">
         <v>8</v>
@@ -8510,7 +8519,7 @@
         <v>226</v>
       </c>
       <c r="F206" s="37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G206" s="37" t="s">
         <v>8</v>
@@ -8540,7 +8549,7 @@
         <v>226</v>
       </c>
       <c r="F207" s="37">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G207" s="37" t="s">
         <v>8</v>
@@ -8570,7 +8579,7 @@
         <v>226</v>
       </c>
       <c r="F208" s="37">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G208" s="37" t="s">
         <v>8</v>
@@ -8600,7 +8609,7 @@
         <v>226</v>
       </c>
       <c r="F209" s="37">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G209" s="37" t="s">
         <v>8</v>
@@ -8612,7 +8621,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="210" spans="1:9" s="52" customFormat="1" ht="61.5" customHeight="1">
+    <row r="210" spans="1:9" ht="17.25">
       <c r="A210" s="9">
         <f t="shared" si="6"/>
         <v>209</v>
@@ -8623,26 +8632,26 @@
       <c r="C210" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D210" s="45" t="s">
+      <c r="D210" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="E210" s="50" t="s">
-        <v>228</v>
-      </c>
-      <c r="F210" s="51">
-        <v>1</v>
-      </c>
-      <c r="G210" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="H210" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="I210" s="52" t="s">
+      <c r="E210" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="F210" s="37">
+        <v>10</v>
+      </c>
+      <c r="G210" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H210" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I210" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="17.25">
+    <row r="211" spans="1:9" s="52" customFormat="1" ht="61.5" customHeight="1">
       <c r="A211" s="9">
         <f t="shared" si="6"/>
         <v>210</v>
@@ -8653,22 +8662,22 @@
       <c r="C211" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D211" s="22" t="s">
+      <c r="D211" s="45" t="s">
         <v>225</v>
       </c>
-      <c r="E211" s="55" t="s">
+      <c r="E211" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="F211" s="37">
-        <v>2</v>
-      </c>
-      <c r="G211" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H211" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I211" s="1" t="s">
+      <c r="F211" s="51">
+        <v>1</v>
+      </c>
+      <c r="G211" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="H211" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I211" s="52" t="s">
         <v>227</v>
       </c>
     </row>
@@ -8690,7 +8699,7 @@
         <v>228</v>
       </c>
       <c r="F212" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G212" s="37" t="s">
         <v>8</v>
@@ -8720,7 +8729,7 @@
         <v>228</v>
       </c>
       <c r="F213" s="37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G213" s="37" t="s">
         <v>8</v>
@@ -8750,7 +8759,7 @@
         <v>228</v>
       </c>
       <c r="F214" s="37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G214" s="37" t="s">
         <v>8</v>
@@ -8780,7 +8789,7 @@
         <v>228</v>
       </c>
       <c r="F215" s="37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G215" s="37" t="s">
         <v>8</v>
@@ -8810,7 +8819,7 @@
         <v>228</v>
       </c>
       <c r="F216" s="37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G216" s="37" t="s">
         <v>8</v>
@@ -8840,7 +8849,7 @@
         <v>228</v>
       </c>
       <c r="F217" s="37">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G217" s="37" t="s">
         <v>8</v>
@@ -8870,7 +8879,7 @@
         <v>228</v>
       </c>
       <c r="F218" s="37">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G218" s="37" t="s">
         <v>8</v>
@@ -8900,7 +8909,7 @@
         <v>228</v>
       </c>
       <c r="F219" s="37">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G219" s="37" t="s">
         <v>8</v>
@@ -8912,7 +8921,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="220" spans="1:9" s="52" customFormat="1" ht="17.25">
+    <row r="220" spans="1:9" ht="17.25">
       <c r="A220" s="9">
         <f t="shared" si="6"/>
         <v>219</v>
@@ -8923,26 +8932,26 @@
       <c r="C220" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D220" s="45" t="s">
-        <v>229</v>
-      </c>
-      <c r="E220" s="50">
-        <v>1</v>
-      </c>
-      <c r="F220" s="50" t="s">
-        <v>230</v>
-      </c>
-      <c r="G220" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="H220" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="I220" s="52" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9" ht="17.25">
+      <c r="D220" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="E220" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="F220" s="37">
+        <v>10</v>
+      </c>
+      <c r="G220" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H220" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I220" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" s="52" customFormat="1" ht="17.25">
       <c r="A221" s="9">
         <f t="shared" si="6"/>
         <v>220</v>
@@ -8953,22 +8962,22 @@
       <c r="C221" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D221" s="42" t="s">
+      <c r="D221" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="E221" s="53">
+      <c r="E221" s="50">
         <v>1</v>
       </c>
-      <c r="F221" s="53" t="s">
-        <v>232</v>
-      </c>
-      <c r="G221" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="H221" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I221" s="1" t="s">
+      <c r="F221" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="G221" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="H221" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I221" s="52" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8990,7 +8999,7 @@
         <v>1</v>
       </c>
       <c r="F222" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G222" s="53" t="s">
         <v>8</v>
@@ -9004,7 +9013,7 @@
     </row>
     <row r="223" spans="1:9" ht="17.25">
       <c r="A223" s="9">
-        <f t="shared" ref="A223:A232" si="7">ROW(A223)-1</f>
+        <f t="shared" si="6"/>
         <v>222</v>
       </c>
       <c r="B223" s="9" t="s">
@@ -9020,7 +9029,7 @@
         <v>1</v>
       </c>
       <c r="F223" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G223" s="53" t="s">
         <v>8</v>
@@ -9034,7 +9043,7 @@
     </row>
     <row r="224" spans="1:9" ht="17.25">
       <c r="A224" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A224:A233" si="7">ROW(A224)-1</f>
         <v>223</v>
       </c>
       <c r="B224" s="9" t="s">
@@ -9047,10 +9056,10 @@
         <v>229</v>
       </c>
       <c r="E224" s="53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F224" s="53" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="G224" s="53" t="s">
         <v>8</v>
@@ -9080,7 +9089,7 @@
         <v>2</v>
       </c>
       <c r="F225" s="53" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G225" s="53" t="s">
         <v>8</v>
@@ -9110,7 +9119,7 @@
         <v>2</v>
       </c>
       <c r="F226" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G226" s="53" t="s">
         <v>8</v>
@@ -9140,7 +9149,7 @@
         <v>2</v>
       </c>
       <c r="F227" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G227" s="53" t="s">
         <v>8</v>
@@ -9167,10 +9176,10 @@
         <v>229</v>
       </c>
       <c r="E228" s="53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F228" s="53" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="G228" s="53" t="s">
         <v>8</v>
@@ -9200,7 +9209,7 @@
         <v>3</v>
       </c>
       <c r="F229" s="53" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G229" s="53" t="s">
         <v>8</v>
@@ -9230,7 +9239,7 @@
         <v>3</v>
       </c>
       <c r="F230" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G230" s="53" t="s">
         <v>8</v>
@@ -9260,7 +9269,7 @@
         <v>3</v>
       </c>
       <c r="F231" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G231" s="53" t="s">
         <v>8</v>
@@ -9272,7 +9281,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="232" spans="1:9" s="52" customFormat="1" ht="17.25">
+    <row r="232" spans="1:9" ht="17.25">
       <c r="A232" s="9">
         <f t="shared" si="7"/>
         <v>231</v>
@@ -9283,22 +9292,52 @@
       <c r="C232" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D232" s="45" t="s">
+      <c r="D232" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="E232" s="53">
+        <v>3</v>
+      </c>
+      <c r="F232" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="G232" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="H232" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I232" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" s="52" customFormat="1" ht="17.25">
+      <c r="A233" s="9">
+        <f t="shared" si="7"/>
+        <v>232</v>
+      </c>
+      <c r="B233" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C233" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D233" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="E232" s="50" t="s">
+      <c r="E233" s="50" t="s">
         <v>236</v>
       </c>
-      <c r="F232" s="50" t="s">
+      <c r="F233" s="50" t="s">
         <v>236</v>
       </c>
-      <c r="G232" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="H232" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="I232" s="52" t="s">
+      <c r="G233" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="H233" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I233" s="52" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>